<commit_message>
Successful generic classification function
</commit_message>
<xml_diff>
--- a/Development/Data/MetaData/MetaDataCCP.xlsx
+++ b/Development/Data/MetaData/MetaDataCCP.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Basti\ARBEIT Lokal\dsCCPhos\Development\MetaData\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Basti\ARBEIT Lokal\dsCCPhos\Development\Data\MetaData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F02D5D3B-F630-43F7-83B9-2466EAB95067}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ED67854E-E684-492A-98DD-E99C1FBE50A4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="2" xr2:uid="{035133D3-9E9F-4CDB-BCDC-A149BB1E9383}"/>
   </bookViews>
@@ -1304,9 +1304,6 @@
     <t>ICDOMorphologyVersion</t>
   </si>
   <si>
-    <t>ICDOMorphology</t>
-  </si>
-  <si>
     <t>ICDOMorphologyCode</t>
   </si>
   <si>
@@ -1515,6 +1512,9 @@
   </si>
   <si>
     <t>Macroscopic Residual Tumor</t>
+  </si>
+  <si>
+    <t>ICDOMorphologyComment</t>
   </si>
 </sst>
 </file>
@@ -1966,10 +1966,10 @@
   <sheetData>
     <row r="1" spans="1:2" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="3" t="s">
-        <v>457</v>
+        <v>456</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>465</v>
+        <v>464</v>
       </c>
     </row>
     <row r="2" spans="1:2" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
@@ -2009,7 +2009,7 @@
         <v>388</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>459</v>
+        <v>458</v>
       </c>
     </row>
     <row r="7" spans="1:2" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
@@ -2017,7 +2017,7 @@
         <v>308</v>
       </c>
       <c r="B7" s="4" t="s">
-        <v>461</v>
+        <v>460</v>
       </c>
     </row>
     <row r="8" spans="1:2" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
@@ -2033,7 +2033,7 @@
         <v>382</v>
       </c>
       <c r="B9" s="4" t="s">
-        <v>458</v>
+        <v>457</v>
       </c>
     </row>
     <row r="10" spans="1:2" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
@@ -2057,7 +2057,7 @@
         <v>361</v>
       </c>
       <c r="B12" s="4" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
     </row>
   </sheetData>
@@ -2073,8 +2073,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CD8BF945-9186-40D3-A998-0B845CD0DDFC}">
   <dimension ref="A1:E103"/>
   <sheetViews>
-    <sheetView topLeftCell="A15" workbookViewId="0">
-      <selection activeCell="E26" sqref="E26"/>
+    <sheetView topLeftCell="A17" workbookViewId="0">
+      <selection activeCell="H31" sqref="H31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="16.33203125" defaultRowHeight="25.2" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -2092,19 +2092,19 @@
   <sheetData>
     <row r="1" spans="1:5" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="3" t="s">
-        <v>457</v>
+        <v>456</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>465</v>
+        <v>464</v>
       </c>
       <c r="C1" s="3" t="s">
         <v>403</v>
       </c>
       <c r="D1" s="3" t="s">
-        <v>460</v>
+        <v>459</v>
       </c>
       <c r="E1" s="3" t="s">
-        <v>468</v>
+        <v>467</v>
       </c>
     </row>
     <row r="2" spans="1:5" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
@@ -2212,7 +2212,7 @@
         <v>314</v>
       </c>
       <c r="E7" s="4" t="s">
-        <v>471</v>
+        <v>470</v>
       </c>
     </row>
     <row r="8" spans="1:5" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
@@ -2338,7 +2338,7 @@
         <v>321</v>
       </c>
       <c r="E14" s="4" t="s">
-        <v>482</v>
+        <v>481</v>
       </c>
     </row>
     <row r="15" spans="1:5" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
@@ -2356,7 +2356,7 @@
         <v>322</v>
       </c>
       <c r="E15" s="4" t="s">
-        <v>483</v>
+        <v>482</v>
       </c>
     </row>
     <row r="16" spans="1:5" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
@@ -2500,7 +2500,7 @@
         <v>329</v>
       </c>
       <c r="E23" s="4" t="s">
-        <v>481</v>
+        <v>480</v>
       </c>
     </row>
     <row r="24" spans="1:5" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
@@ -2518,7 +2518,7 @@
         <v>330</v>
       </c>
       <c r="E24" s="4" t="s">
-        <v>472</v>
+        <v>471</v>
       </c>
     </row>
     <row r="25" spans="1:5" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
@@ -2536,7 +2536,7 @@
         <v>331</v>
       </c>
       <c r="E25" s="4" t="s">
-        <v>490</v>
+        <v>489</v>
       </c>
     </row>
     <row r="26" spans="1:5" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
@@ -2554,7 +2554,7 @@
         <v>332</v>
       </c>
       <c r="E26" s="4" t="s">
-        <v>484</v>
+        <v>483</v>
       </c>
     </row>
     <row r="27" spans="1:5" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
@@ -2572,7 +2572,7 @@
         <v>333</v>
       </c>
       <c r="E27" s="4" t="s">
-        <v>485</v>
+        <v>484</v>
       </c>
     </row>
     <row r="28" spans="1:5" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
@@ -2590,7 +2590,7 @@
         <v>334</v>
       </c>
       <c r="E28" s="4" t="s">
-        <v>486</v>
+        <v>485</v>
       </c>
     </row>
     <row r="29" spans="1:5" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
@@ -2662,7 +2662,7 @@
         <v>337</v>
       </c>
       <c r="E32" s="4" t="s">
-        <v>473</v>
+        <v>472</v>
       </c>
     </row>
     <row r="33" spans="1:5" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
@@ -2716,7 +2716,7 @@
         <v>340</v>
       </c>
       <c r="E35" s="4" t="s">
-        <v>423</v>
+        <v>492</v>
       </c>
     </row>
     <row r="36" spans="1:5" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
@@ -2806,7 +2806,7 @@
         <v>344</v>
       </c>
       <c r="E40" s="4" t="s">
-        <v>470</v>
+        <v>469</v>
       </c>
     </row>
     <row r="41" spans="1:5" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
@@ -2824,7 +2824,7 @@
         <v>345</v>
       </c>
       <c r="E41" s="4" t="s">
-        <v>487</v>
+        <v>486</v>
       </c>
     </row>
     <row r="42" spans="1:5" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
@@ -2842,7 +2842,7 @@
         <v>346</v>
       </c>
       <c r="E42" s="4" t="s">
-        <v>488</v>
+        <v>487</v>
       </c>
     </row>
     <row r="43" spans="1:5" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
@@ -2860,7 +2860,7 @@
         <v>348</v>
       </c>
       <c r="E43" s="4" t="s">
-        <v>424</v>
+        <v>423</v>
       </c>
     </row>
     <row r="44" spans="1:5" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
@@ -2914,7 +2914,7 @@
         <v>349</v>
       </c>
       <c r="E46" s="4" t="s">
-        <v>489</v>
+        <v>488</v>
       </c>
     </row>
     <row r="47" spans="1:5" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
@@ -3058,7 +3058,7 @@
         <v>357</v>
       </c>
       <c r="E54" s="4" t="s">
-        <v>476</v>
+        <v>475</v>
       </c>
     </row>
     <row r="55" spans="1:5" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
@@ -3076,7 +3076,7 @@
         <v>358</v>
       </c>
       <c r="E55" s="4" t="s">
-        <v>425</v>
+        <v>424</v>
       </c>
     </row>
     <row r="56" spans="1:5" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
@@ -3094,7 +3094,7 @@
         <v>359</v>
       </c>
       <c r="E56" s="4" t="s">
-        <v>426</v>
+        <v>425</v>
       </c>
     </row>
     <row r="57" spans="1:5" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
@@ -3112,7 +3112,7 @@
         <v>360</v>
       </c>
       <c r="E57" s="4" t="s">
-        <v>427</v>
+        <v>426</v>
       </c>
     </row>
     <row r="58" spans="1:5" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
@@ -3130,7 +3130,7 @@
         <v>362</v>
       </c>
       <c r="E58" s="4" t="s">
-        <v>428</v>
+        <v>427</v>
       </c>
     </row>
     <row r="59" spans="1:5" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
@@ -3184,7 +3184,7 @@
         <v>363</v>
       </c>
       <c r="E61" s="4" t="s">
-        <v>441</v>
+        <v>440</v>
       </c>
     </row>
     <row r="62" spans="1:5" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
@@ -3202,7 +3202,7 @@
         <v>364</v>
       </c>
       <c r="E62" s="4" t="s">
-        <v>475</v>
+        <v>474</v>
       </c>
     </row>
     <row r="63" spans="1:5" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
@@ -3220,7 +3220,7 @@
         <v>365</v>
       </c>
       <c r="E63" s="4" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
     </row>
     <row r="64" spans="1:5" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
@@ -3238,7 +3238,7 @@
         <v>366</v>
       </c>
       <c r="E64" s="4" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
     </row>
     <row r="65" spans="1:5" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
@@ -3256,7 +3256,7 @@
         <v>367</v>
       </c>
       <c r="E65" s="4" t="s">
-        <v>432</v>
+        <v>431</v>
       </c>
     </row>
     <row r="66" spans="1:5" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
@@ -3274,7 +3274,7 @@
         <v>368</v>
       </c>
       <c r="E66" s="4" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
     </row>
     <row r="67" spans="1:5" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
@@ -3292,7 +3292,7 @@
         <v>369</v>
       </c>
       <c r="E67" s="4" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
     </row>
     <row r="68" spans="1:5" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
@@ -3310,7 +3310,7 @@
         <v>370</v>
       </c>
       <c r="E68" s="4" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
     </row>
     <row r="69" spans="1:5" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
@@ -3328,7 +3328,7 @@
         <v>371</v>
       </c>
       <c r="E69" s="4" t="s">
-        <v>469</v>
+        <v>468</v>
       </c>
     </row>
     <row r="70" spans="1:5" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
@@ -3346,7 +3346,7 @@
         <v>372</v>
       </c>
       <c r="E70" s="4" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
     </row>
     <row r="71" spans="1:5" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
@@ -3364,7 +3364,7 @@
         <v>373</v>
       </c>
       <c r="E71" s="4" t="s">
-        <v>437</v>
+        <v>436</v>
       </c>
     </row>
     <row r="72" spans="1:5" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
@@ -3382,7 +3382,7 @@
         <v>374</v>
       </c>
       <c r="E72" s="4" t="s">
-        <v>438</v>
+        <v>437</v>
       </c>
     </row>
     <row r="73" spans="1:5" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
@@ -3454,7 +3454,7 @@
         <v>377</v>
       </c>
       <c r="E76" s="4" t="s">
-        <v>439</v>
+        <v>438</v>
       </c>
     </row>
     <row r="77" spans="1:5" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
@@ -3472,7 +3472,7 @@
         <v>378</v>
       </c>
       <c r="E77" s="4" t="s">
-        <v>440</v>
+        <v>439</v>
       </c>
     </row>
     <row r="78" spans="1:5" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
@@ -3544,7 +3544,7 @@
         <v>383</v>
       </c>
       <c r="E81" s="4" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
     </row>
     <row r="82" spans="1:5" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
@@ -3598,7 +3598,7 @@
         <v>384</v>
       </c>
       <c r="E84" s="4" t="s">
-        <v>443</v>
+        <v>442</v>
       </c>
     </row>
     <row r="85" spans="1:5" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
@@ -3616,7 +3616,7 @@
         <v>385</v>
       </c>
       <c r="E85" s="4" t="s">
-        <v>444</v>
+        <v>443</v>
       </c>
     </row>
     <row r="86" spans="1:5" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
@@ -3634,7 +3634,7 @@
         <v>386</v>
       </c>
       <c r="E86" s="4" t="s">
-        <v>445</v>
+        <v>444</v>
       </c>
     </row>
     <row r="87" spans="1:5" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
@@ -3652,7 +3652,7 @@
         <v>387</v>
       </c>
       <c r="E87" s="4" t="s">
-        <v>446</v>
+        <v>445</v>
       </c>
     </row>
     <row r="88" spans="1:5" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
@@ -3670,7 +3670,7 @@
         <v>389</v>
       </c>
       <c r="E88" s="4" t="s">
-        <v>447</v>
+        <v>446</v>
       </c>
     </row>
     <row r="89" spans="1:5" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
@@ -3724,7 +3724,7 @@
         <v>390</v>
       </c>
       <c r="E91" s="4" t="s">
-        <v>448</v>
+        <v>447</v>
       </c>
     </row>
     <row r="92" spans="1:5" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
@@ -3742,7 +3742,7 @@
         <v>391</v>
       </c>
       <c r="E92" s="4" t="s">
-        <v>449</v>
+        <v>448</v>
       </c>
     </row>
     <row r="93" spans="1:5" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
@@ -3760,7 +3760,7 @@
         <v>392</v>
       </c>
       <c r="E93" s="4" t="s">
-        <v>450</v>
+        <v>449</v>
       </c>
     </row>
     <row r="94" spans="1:5" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
@@ -3778,7 +3778,7 @@
         <v>393</v>
       </c>
       <c r="E94" s="4" t="s">
-        <v>456</v>
+        <v>455</v>
       </c>
     </row>
     <row r="95" spans="1:5" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
@@ -3832,7 +3832,7 @@
         <v>396</v>
       </c>
       <c r="E97" s="4" t="s">
-        <v>474</v>
+        <v>473</v>
       </c>
     </row>
     <row r="98" spans="1:5" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
@@ -3868,7 +3868,7 @@
         <v>398</v>
       </c>
       <c r="E99" s="4" t="s">
-        <v>451</v>
+        <v>450</v>
       </c>
     </row>
     <row r="100" spans="1:5" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
@@ -3886,7 +3886,7 @@
         <v>399</v>
       </c>
       <c r="E100" s="4" t="s">
-        <v>452</v>
+        <v>451</v>
       </c>
     </row>
     <row r="101" spans="1:5" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
@@ -3904,7 +3904,7 @@
         <v>400</v>
       </c>
       <c r="E101" s="4" t="s">
-        <v>453</v>
+        <v>452</v>
       </c>
     </row>
     <row r="102" spans="1:5" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
@@ -3922,7 +3922,7 @@
         <v>401</v>
       </c>
       <c r="E102" s="4" t="s">
-        <v>454</v>
+        <v>453</v>
       </c>
     </row>
     <row r="103" spans="1:5" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
@@ -3940,7 +3940,7 @@
         <v>402</v>
       </c>
       <c r="E103" s="4" t="s">
-        <v>455</v>
+        <v>454</v>
       </c>
     </row>
   </sheetData>
@@ -3954,10 +3954,10 @@
   <dimension ref="A1:L256"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="D2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="1" topLeftCell="D14" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="G9" sqref="G9"/>
+      <selection pane="bottomRight" activeCell="G22" sqref="G22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="16.33203125" defaultRowHeight="25.2" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -3978,25 +3978,25 @@
   <sheetData>
     <row r="1" spans="1:8" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="3" t="s">
-        <v>465</v>
+        <v>464</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>462</v>
+        <v>461</v>
       </c>
       <c r="C1" s="3" t="s">
         <v>193</v>
       </c>
       <c r="D1" s="3" t="s">
+        <v>462</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>465</v>
+      </c>
+      <c r="F1" s="7" t="s">
+        <v>466</v>
+      </c>
+      <c r="G1" s="2" t="s">
         <v>463</v>
-      </c>
-      <c r="E1" s="3" t="s">
-        <v>466</v>
-      </c>
-      <c r="F1" s="7" t="s">
-        <v>467</v>
-      </c>
-      <c r="G1" s="2" t="s">
-        <v>464</v>
       </c>
       <c r="H1" s="3" t="s">
         <v>194</v>
@@ -7759,13 +7759,13 @@
         <v>195</v>
       </c>
       <c r="D159" s="4" t="s">
+        <v>478</v>
+      </c>
+      <c r="E159" s="4" t="s">
+        <v>478</v>
+      </c>
+      <c r="F159" s="8" t="s">
         <v>479</v>
-      </c>
-      <c r="E159" s="4" t="s">
-        <v>479</v>
-      </c>
-      <c r="F159" s="8" t="s">
-        <v>480</v>
       </c>
     </row>
     <row r="160" spans="1:8" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
@@ -8761,13 +8761,13 @@
         <v>195</v>
       </c>
       <c r="D201" s="4" t="s">
+        <v>476</v>
+      </c>
+      <c r="E201" s="4" t="s">
+        <v>476</v>
+      </c>
+      <c r="F201" s="8" t="s">
         <v>477</v>
-      </c>
-      <c r="E201" s="4" t="s">
-        <v>477</v>
-      </c>
-      <c r="F201" s="8" t="s">
-        <v>478</v>
       </c>
       <c r="J201" s="5"/>
     </row>
@@ -9590,7 +9590,7 @@
         <v>261</v>
       </c>
       <c r="F236" s="8" t="s">
-        <v>492</v>
+        <v>491</v>
       </c>
       <c r="G236" s="5" t="s">
         <v>262</v>
@@ -10039,7 +10039,7 @@
         <v>46</v>
       </c>
       <c r="F253" s="9" t="s">
-        <v>491</v>
+        <v>490</v>
       </c>
       <c r="G253" s="5"/>
       <c r="J253" s="5"/>

</xml_diff>

<commit_message>
Restructured data transformation function
</commit_message>
<xml_diff>
--- a/Development/Data/MetaData/MetaDataCCP.xlsx
+++ b/Development/Data/MetaData/MetaDataCCP.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Basti\ARBEIT Lokal\dsCCPhos\Development\Data\MetaData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ED67854E-E684-492A-98DD-E99C1FBE50A4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{252E6955-6951-4EFC-BCFA-FC0377068A83}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="2" xr2:uid="{035133D3-9E9F-4CDB-BCDC-A149BB1E9383}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{035133D3-9E9F-4CDB-BCDC-A149BB1E9383}"/>
   </bookViews>
   <sheets>
     <sheet name="TableNames" sheetId="11" r:id="rId1"/>
@@ -1127,9 +1127,6 @@
     <t>system-therapy-id</t>
   </si>
   <si>
-    <t>systemische_therapie_stellung_zu_operativer_therapie</t>
-  </si>
-  <si>
     <t>intention_chemotherapie</t>
   </si>
   <si>
@@ -1515,6 +1512,9 @@
   </si>
   <si>
     <t>ICDOMorphologyComment</t>
+  </si>
+  <si>
+    <t>systemische_therapie_stellung_zu_op_therapie</t>
   </si>
 </sst>
 </file>
@@ -1966,15 +1966,15 @@
   <sheetData>
     <row r="1" spans="1:2" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="3" t="s">
-        <v>456</v>
+        <v>455</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>464</v>
+        <v>463</v>
       </c>
     </row>
     <row r="2" spans="1:2" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="4" t="s">
-        <v>394</v>
+        <v>393</v>
       </c>
       <c r="B2" s="4" t="s">
         <v>277</v>
@@ -2006,10 +2006,10 @@
     </row>
     <row r="6" spans="1:2" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="4" t="s">
-        <v>388</v>
+        <v>387</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>458</v>
+        <v>457</v>
       </c>
     </row>
     <row r="7" spans="1:2" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
@@ -2017,7 +2017,7 @@
         <v>308</v>
       </c>
       <c r="B7" s="4" t="s">
-        <v>460</v>
+        <v>459</v>
       </c>
     </row>
     <row r="8" spans="1:2" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
@@ -2030,10 +2030,10 @@
     </row>
     <row r="9" spans="1:2" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="4" t="s">
-        <v>382</v>
+        <v>381</v>
       </c>
       <c r="B9" s="4" t="s">
-        <v>457</v>
+        <v>456</v>
       </c>
     </row>
     <row r="10" spans="1:2" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
@@ -2046,7 +2046,7 @@
     </row>
     <row r="11" spans="1:2" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A11" s="4" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
       <c r="B11" s="4" t="s">
         <v>255</v>
@@ -2057,7 +2057,7 @@
         <v>361</v>
       </c>
       <c r="B12" s="4" t="s">
-        <v>428</v>
+        <v>427</v>
       </c>
     </row>
   </sheetData>
@@ -2073,8 +2073,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CD8BF945-9186-40D3-A998-0B845CD0DDFC}">
   <dimension ref="A1:E103"/>
   <sheetViews>
-    <sheetView topLeftCell="A17" workbookViewId="0">
-      <selection activeCell="H31" sqref="H31"/>
+    <sheetView tabSelected="1" topLeftCell="A51" workbookViewId="0">
+      <selection activeCell="F57" sqref="F57"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="16.33203125" defaultRowHeight="25.2" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -2092,19 +2092,19 @@
   <sheetData>
     <row r="1" spans="1:5" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="3" t="s">
-        <v>456</v>
+        <v>455</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>464</v>
+        <v>463</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>403</v>
+        <v>402</v>
       </c>
       <c r="D1" s="3" t="s">
-        <v>459</v>
+        <v>458</v>
       </c>
       <c r="E1" s="3" t="s">
-        <v>467</v>
+        <v>466</v>
       </c>
     </row>
     <row r="2" spans="1:5" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
@@ -2122,7 +2122,7 @@
         <v>309</v>
       </c>
       <c r="E2" s="4" t="s">
-        <v>404</v>
+        <v>403</v>
       </c>
     </row>
     <row r="3" spans="1:5" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
@@ -2140,7 +2140,7 @@
         <v>310</v>
       </c>
       <c r="E3" s="4" t="s">
-        <v>406</v>
+        <v>405</v>
       </c>
     </row>
     <row r="4" spans="1:5" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
@@ -2158,7 +2158,7 @@
         <v>311</v>
       </c>
       <c r="E4" s="4" t="s">
-        <v>407</v>
+        <v>406</v>
       </c>
     </row>
     <row r="5" spans="1:5" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
@@ -2176,7 +2176,7 @@
         <v>312</v>
       </c>
       <c r="E5" s="4" t="s">
-        <v>408</v>
+        <v>407</v>
       </c>
     </row>
     <row r="6" spans="1:5" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
@@ -2194,7 +2194,7 @@
         <v>313</v>
       </c>
       <c r="E6" s="4" t="s">
-        <v>409</v>
+        <v>408</v>
       </c>
     </row>
     <row r="7" spans="1:5" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
@@ -2212,7 +2212,7 @@
         <v>314</v>
       </c>
       <c r="E7" s="4" t="s">
-        <v>470</v>
+        <v>469</v>
       </c>
     </row>
     <row r="8" spans="1:5" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
@@ -2248,7 +2248,7 @@
         <v>316</v>
       </c>
       <c r="E9" s="4" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
     </row>
     <row r="10" spans="1:5" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
@@ -2266,7 +2266,7 @@
         <v>317</v>
       </c>
       <c r="E10" s="4" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
     </row>
     <row r="11" spans="1:5" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
@@ -2284,7 +2284,7 @@
         <v>319</v>
       </c>
       <c r="E11" s="4" t="s">
-        <v>405</v>
+        <v>404</v>
       </c>
     </row>
     <row r="12" spans="1:5" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
@@ -2302,7 +2302,7 @@
         <v>309</v>
       </c>
       <c r="E12" s="4" t="s">
-        <v>404</v>
+        <v>403</v>
       </c>
     </row>
     <row r="13" spans="1:5" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
@@ -2320,7 +2320,7 @@
         <v>320</v>
       </c>
       <c r="E13" s="4" t="s">
-        <v>415</v>
+        <v>414</v>
       </c>
     </row>
     <row r="14" spans="1:5" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
@@ -2338,7 +2338,7 @@
         <v>321</v>
       </c>
       <c r="E14" s="4" t="s">
-        <v>481</v>
+        <v>480</v>
       </c>
     </row>
     <row r="15" spans="1:5" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
@@ -2356,7 +2356,7 @@
         <v>322</v>
       </c>
       <c r="E15" s="4" t="s">
-        <v>482</v>
+        <v>481</v>
       </c>
     </row>
     <row r="16" spans="1:5" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
@@ -2374,7 +2374,7 @@
         <v>323</v>
       </c>
       <c r="E16" s="4" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
     </row>
     <row r="17" spans="1:5" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
@@ -2392,7 +2392,7 @@
         <v>324</v>
       </c>
       <c r="E17" s="4" t="s">
-        <v>414</v>
+        <v>413</v>
       </c>
     </row>
     <row r="18" spans="1:5" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
@@ -2410,7 +2410,7 @@
         <v>325</v>
       </c>
       <c r="E18" s="4" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
     </row>
     <row r="19" spans="1:5" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
@@ -2446,7 +2446,7 @@
         <v>328</v>
       </c>
       <c r="E20" s="4" t="s">
-        <v>416</v>
+        <v>415</v>
       </c>
     </row>
     <row r="21" spans="1:5" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
@@ -2464,7 +2464,7 @@
         <v>319</v>
       </c>
       <c r="E21" s="4" t="s">
-        <v>405</v>
+        <v>404</v>
       </c>
     </row>
     <row r="22" spans="1:5" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
@@ -2482,7 +2482,7 @@
         <v>309</v>
       </c>
       <c r="E22" s="4" t="s">
-        <v>404</v>
+        <v>403</v>
       </c>
     </row>
     <row r="23" spans="1:5" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
@@ -2500,7 +2500,7 @@
         <v>329</v>
       </c>
       <c r="E23" s="4" t="s">
-        <v>480</v>
+        <v>479</v>
       </c>
     </row>
     <row r="24" spans="1:5" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
@@ -2518,7 +2518,7 @@
         <v>330</v>
       </c>
       <c r="E24" s="4" t="s">
-        <v>471</v>
+        <v>470</v>
       </c>
     </row>
     <row r="25" spans="1:5" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
@@ -2536,7 +2536,7 @@
         <v>331</v>
       </c>
       <c r="E25" s="4" t="s">
-        <v>489</v>
+        <v>488</v>
       </c>
     </row>
     <row r="26" spans="1:5" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
@@ -2554,7 +2554,7 @@
         <v>332</v>
       </c>
       <c r="E26" s="4" t="s">
-        <v>483</v>
+        <v>482</v>
       </c>
     </row>
     <row r="27" spans="1:5" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
@@ -2572,7 +2572,7 @@
         <v>333</v>
       </c>
       <c r="E27" s="4" t="s">
-        <v>484</v>
+        <v>483</v>
       </c>
     </row>
     <row r="28" spans="1:5" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
@@ -2590,7 +2590,7 @@
         <v>334</v>
       </c>
       <c r="E28" s="4" t="s">
-        <v>485</v>
+        <v>484</v>
       </c>
     </row>
     <row r="29" spans="1:5" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
@@ -2608,7 +2608,7 @@
         <v>336</v>
       </c>
       <c r="E29" s="4" t="s">
-        <v>417</v>
+        <v>416</v>
       </c>
     </row>
     <row r="30" spans="1:5" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
@@ -2626,7 +2626,7 @@
         <v>319</v>
       </c>
       <c r="E30" s="4" t="s">
-        <v>405</v>
+        <v>404</v>
       </c>
     </row>
     <row r="31" spans="1:5" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
@@ -2644,7 +2644,7 @@
         <v>309</v>
       </c>
       <c r="E31" s="4" t="s">
-        <v>404</v>
+        <v>403</v>
       </c>
     </row>
     <row r="32" spans="1:5" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
@@ -2662,7 +2662,7 @@
         <v>337</v>
       </c>
       <c r="E32" s="4" t="s">
-        <v>472</v>
+        <v>471</v>
       </c>
     </row>
     <row r="33" spans="1:5" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
@@ -2680,7 +2680,7 @@
         <v>338</v>
       </c>
       <c r="E33" s="4" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
     </row>
     <row r="34" spans="1:5" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
@@ -2698,7 +2698,7 @@
         <v>339</v>
       </c>
       <c r="E34" s="4" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
     </row>
     <row r="35" spans="1:5" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
@@ -2716,7 +2716,7 @@
         <v>340</v>
       </c>
       <c r="E35" s="4" t="s">
-        <v>492</v>
+        <v>491</v>
       </c>
     </row>
     <row r="36" spans="1:5" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
@@ -2752,7 +2752,7 @@
         <v>343</v>
       </c>
       <c r="E37" s="4" t="s">
-        <v>418</v>
+        <v>417</v>
       </c>
     </row>
     <row r="38" spans="1:5" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
@@ -2770,7 +2770,7 @@
         <v>319</v>
       </c>
       <c r="E38" s="4" t="s">
-        <v>405</v>
+        <v>404</v>
       </c>
     </row>
     <row r="39" spans="1:5" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
@@ -2788,7 +2788,7 @@
         <v>309</v>
       </c>
       <c r="E39" s="4" t="s">
-        <v>404</v>
+        <v>403</v>
       </c>
     </row>
     <row r="40" spans="1:5" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
@@ -2806,7 +2806,7 @@
         <v>344</v>
       </c>
       <c r="E40" s="4" t="s">
-        <v>469</v>
+        <v>468</v>
       </c>
     </row>
     <row r="41" spans="1:5" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
@@ -2824,7 +2824,7 @@
         <v>345</v>
       </c>
       <c r="E41" s="4" t="s">
-        <v>486</v>
+        <v>485</v>
       </c>
     </row>
     <row r="42" spans="1:5" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
@@ -2842,7 +2842,7 @@
         <v>346</v>
       </c>
       <c r="E42" s="4" t="s">
-        <v>487</v>
+        <v>486</v>
       </c>
     </row>
     <row r="43" spans="1:5" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
@@ -2860,7 +2860,7 @@
         <v>348</v>
       </c>
       <c r="E43" s="4" t="s">
-        <v>423</v>
+        <v>422</v>
       </c>
     </row>
     <row r="44" spans="1:5" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
@@ -2878,7 +2878,7 @@
         <v>319</v>
       </c>
       <c r="E44" s="4" t="s">
-        <v>405</v>
+        <v>404</v>
       </c>
     </row>
     <row r="45" spans="1:5" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
@@ -2896,7 +2896,7 @@
         <v>309</v>
       </c>
       <c r="E45" s="4" t="s">
-        <v>404</v>
+        <v>403</v>
       </c>
     </row>
     <row r="46" spans="1:5" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
@@ -2914,7 +2914,7 @@
         <v>349</v>
       </c>
       <c r="E46" s="4" t="s">
-        <v>488</v>
+        <v>487</v>
       </c>
     </row>
     <row r="47" spans="1:5" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
@@ -3058,7 +3058,7 @@
         <v>357</v>
       </c>
       <c r="E54" s="4" t="s">
-        <v>475</v>
+        <v>474</v>
       </c>
     </row>
     <row r="55" spans="1:5" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
@@ -3076,7 +3076,7 @@
         <v>358</v>
       </c>
       <c r="E55" s="4" t="s">
-        <v>424</v>
+        <v>423</v>
       </c>
     </row>
     <row r="56" spans="1:5" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
@@ -3094,7 +3094,7 @@
         <v>359</v>
       </c>
       <c r="E56" s="4" t="s">
-        <v>425</v>
+        <v>424</v>
       </c>
     </row>
     <row r="57" spans="1:5" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
@@ -3112,7 +3112,7 @@
         <v>360</v>
       </c>
       <c r="E57" s="4" t="s">
-        <v>426</v>
+        <v>425</v>
       </c>
     </row>
     <row r="58" spans="1:5" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
@@ -3130,7 +3130,7 @@
         <v>362</v>
       </c>
       <c r="E58" s="4" t="s">
-        <v>427</v>
+        <v>426</v>
       </c>
     </row>
     <row r="59" spans="1:5" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
@@ -3148,7 +3148,7 @@
         <v>319</v>
       </c>
       <c r="E59" s="4" t="s">
-        <v>405</v>
+        <v>404</v>
       </c>
     </row>
     <row r="60" spans="1:5" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
@@ -3166,7 +3166,7 @@
         <v>309</v>
       </c>
       <c r="E60" s="4" t="s">
-        <v>404</v>
+        <v>403</v>
       </c>
     </row>
     <row r="61" spans="1:5" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
@@ -3181,10 +3181,10 @@
         <v>4</v>
       </c>
       <c r="D61" s="4" t="s">
-        <v>363</v>
+        <v>492</v>
       </c>
       <c r="E61" s="4" t="s">
-        <v>440</v>
+        <v>439</v>
       </c>
     </row>
     <row r="62" spans="1:5" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
@@ -3199,10 +3199,10 @@
         <v>5</v>
       </c>
       <c r="D62" s="4" t="s">
-        <v>364</v>
+        <v>363</v>
       </c>
       <c r="E62" s="4" t="s">
-        <v>474</v>
+        <v>473</v>
       </c>
     </row>
     <row r="63" spans="1:5" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
@@ -3217,10 +3217,10 @@
         <v>6</v>
       </c>
       <c r="D63" s="4" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
       <c r="E63" s="4" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
     </row>
     <row r="64" spans="1:5" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
@@ -3235,10 +3235,10 @@
         <v>7</v>
       </c>
       <c r="D64" s="4" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
       <c r="E64" s="4" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
     </row>
     <row r="65" spans="1:5" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
@@ -3253,10 +3253,10 @@
         <v>8</v>
       </c>
       <c r="D65" s="4" t="s">
-        <v>367</v>
+        <v>366</v>
       </c>
       <c r="E65" s="4" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
     </row>
     <row r="66" spans="1:5" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
@@ -3271,10 +3271,10 @@
         <v>9</v>
       </c>
       <c r="D66" s="4" t="s">
-        <v>368</v>
+        <v>367</v>
       </c>
       <c r="E66" s="4" t="s">
-        <v>432</v>
+        <v>431</v>
       </c>
     </row>
     <row r="67" spans="1:5" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
@@ -3289,10 +3289,10 @@
         <v>10</v>
       </c>
       <c r="D67" s="4" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
       <c r="E67" s="4" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
     </row>
     <row r="68" spans="1:5" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
@@ -3307,10 +3307,10 @@
         <v>11</v>
       </c>
       <c r="D68" s="4" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
       <c r="E68" s="4" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
     </row>
     <row r="69" spans="1:5" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
@@ -3325,10 +3325,10 @@
         <v>12</v>
       </c>
       <c r="D69" s="4" t="s">
-        <v>371</v>
+        <v>370</v>
       </c>
       <c r="E69" s="4" t="s">
-        <v>468</v>
+        <v>467</v>
       </c>
     </row>
     <row r="70" spans="1:5" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
@@ -3343,10 +3343,10 @@
         <v>13</v>
       </c>
       <c r="D70" s="4" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
       <c r="E70" s="4" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
     </row>
     <row r="71" spans="1:5" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
@@ -3361,10 +3361,10 @@
         <v>14</v>
       </c>
       <c r="D71" s="4" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
       <c r="E71" s="4" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
     </row>
     <row r="72" spans="1:5" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
@@ -3379,15 +3379,15 @@
         <v>15</v>
       </c>
       <c r="D72" s="4" t="s">
-        <v>374</v>
+        <v>373</v>
       </c>
       <c r="E72" s="4" t="s">
-        <v>437</v>
+        <v>436</v>
       </c>
     </row>
     <row r="73" spans="1:5" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A73" s="4" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
       <c r="B73" s="4" t="str">
         <f>VLOOKUP(A73,TableNames!$A$2:$B$12,2,FALSE)</f>
@@ -3397,15 +3397,15 @@
         <v>1</v>
       </c>
       <c r="D73" s="4" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
       <c r="E73" s="4" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
     </row>
     <row r="74" spans="1:5" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A74" s="4" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
       <c r="B74" s="4" t="str">
         <f>VLOOKUP(A74,TableNames!$A$2:$B$12,2,FALSE)</f>
@@ -3418,12 +3418,12 @@
         <v>319</v>
       </c>
       <c r="E74" s="4" t="s">
-        <v>405</v>
+        <v>404</v>
       </c>
     </row>
     <row r="75" spans="1:5" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A75" s="4" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
       <c r="B75" s="4" t="str">
         <f>VLOOKUP(A75,TableNames!$A$2:$B$12,2,FALSE)</f>
@@ -3436,12 +3436,12 @@
         <v>309</v>
       </c>
       <c r="E75" s="4" t="s">
-        <v>404</v>
+        <v>403</v>
       </c>
     </row>
     <row r="76" spans="1:5" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A76" s="4" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
       <c r="B76" s="4" t="str">
         <f>VLOOKUP(A76,TableNames!$A$2:$B$12,2,FALSE)</f>
@@ -3451,15 +3451,15 @@
         <v>4</v>
       </c>
       <c r="D76" s="4" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
       <c r="E76" s="4" t="s">
-        <v>438</v>
+        <v>437</v>
       </c>
     </row>
     <row r="77" spans="1:5" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A77" s="4" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
       <c r="B77" s="4" t="str">
         <f>VLOOKUP(A77,TableNames!$A$2:$B$12,2,FALSE)</f>
@@ -3469,15 +3469,15 @@
         <v>5</v>
       </c>
       <c r="D77" s="4" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="E77" s="4" t="s">
-        <v>439</v>
+        <v>438</v>
       </c>
     </row>
     <row r="78" spans="1:5" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A78" s="4" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
       <c r="B78" s="4" t="str">
         <f>VLOOKUP(A78,TableNames!$A$2:$B$12,2,FALSE)</f>
@@ -3487,7 +3487,7 @@
         <v>6</v>
       </c>
       <c r="D78" s="4" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
       <c r="E78" s="4" t="s">
         <v>173</v>
@@ -3495,7 +3495,7 @@
     </row>
     <row r="79" spans="1:5" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A79" s="4" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
       <c r="B79" s="4" t="str">
         <f>VLOOKUP(A79,TableNames!$A$2:$B$12,2,FALSE)</f>
@@ -3505,7 +3505,7 @@
         <v>7</v>
       </c>
       <c r="D79" s="4" t="s">
-        <v>380</v>
+        <v>379</v>
       </c>
       <c r="E79" s="4" t="s">
         <v>256</v>
@@ -3513,7 +3513,7 @@
     </row>
     <row r="80" spans="1:5" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A80" s="4" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
       <c r="B80" s="4" t="str">
         <f>VLOOKUP(A80,TableNames!$A$2:$B$12,2,FALSE)</f>
@@ -3523,7 +3523,7 @@
         <v>8</v>
       </c>
       <c r="D80" s="4" t="s">
-        <v>381</v>
+        <v>380</v>
       </c>
       <c r="E80" s="4" t="s">
         <v>274</v>
@@ -3531,7 +3531,7 @@
     </row>
     <row r="81" spans="1:5" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A81" s="4" t="s">
-        <v>382</v>
+        <v>381</v>
       </c>
       <c r="B81" s="4" t="str">
         <f>VLOOKUP(A81,TableNames!$A$2:$B$12,2,FALSE)</f>
@@ -3541,15 +3541,15 @@
         <v>1</v>
       </c>
       <c r="D81" s="4" t="s">
-        <v>383</v>
+        <v>382</v>
       </c>
       <c r="E81" s="4" t="s">
-        <v>441</v>
+        <v>440</v>
       </c>
     </row>
     <row r="82" spans="1:5" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A82" s="4" t="s">
-        <v>382</v>
+        <v>381</v>
       </c>
       <c r="B82" s="4" t="str">
         <f>VLOOKUP(A82,TableNames!$A$2:$B$12,2,FALSE)</f>
@@ -3562,12 +3562,12 @@
         <v>319</v>
       </c>
       <c r="E82" s="4" t="s">
-        <v>405</v>
+        <v>404</v>
       </c>
     </row>
     <row r="83" spans="1:5" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A83" s="4" t="s">
-        <v>382</v>
+        <v>381</v>
       </c>
       <c r="B83" s="4" t="str">
         <f>VLOOKUP(A83,TableNames!$A$2:$B$12,2,FALSE)</f>
@@ -3580,12 +3580,12 @@
         <v>309</v>
       </c>
       <c r="E83" s="4" t="s">
-        <v>404</v>
+        <v>403</v>
       </c>
     </row>
     <row r="84" spans="1:5" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A84" s="4" t="s">
-        <v>382</v>
+        <v>381</v>
       </c>
       <c r="B84" s="4" t="str">
         <f>VLOOKUP(A84,TableNames!$A$2:$B$12,2,FALSE)</f>
@@ -3595,15 +3595,15 @@
         <v>4</v>
       </c>
       <c r="D84" s="4" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
       <c r="E84" s="4" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
     </row>
     <row r="85" spans="1:5" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A85" s="4" t="s">
-        <v>382</v>
+        <v>381</v>
       </c>
       <c r="B85" s="4" t="str">
         <f>VLOOKUP(A85,TableNames!$A$2:$B$12,2,FALSE)</f>
@@ -3613,15 +3613,15 @@
         <v>5</v>
       </c>
       <c r="D85" s="4" t="s">
-        <v>385</v>
+        <v>384</v>
       </c>
       <c r="E85" s="4" t="s">
-        <v>443</v>
+        <v>442</v>
       </c>
     </row>
     <row r="86" spans="1:5" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A86" s="4" t="s">
-        <v>382</v>
+        <v>381</v>
       </c>
       <c r="B86" s="4" t="str">
         <f>VLOOKUP(A86,TableNames!$A$2:$B$12,2,FALSE)</f>
@@ -3631,15 +3631,15 @@
         <v>6</v>
       </c>
       <c r="D86" s="4" t="s">
-        <v>386</v>
+        <v>385</v>
       </c>
       <c r="E86" s="4" t="s">
-        <v>444</v>
+        <v>443</v>
       </c>
     </row>
     <row r="87" spans="1:5" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A87" s="4" t="s">
-        <v>382</v>
+        <v>381</v>
       </c>
       <c r="B87" s="4" t="str">
         <f>VLOOKUP(A87,TableNames!$A$2:$B$12,2,FALSE)</f>
@@ -3649,15 +3649,15 @@
         <v>7</v>
       </c>
       <c r="D87" s="4" t="s">
-        <v>387</v>
+        <v>386</v>
       </c>
       <c r="E87" s="4" t="s">
-        <v>445</v>
+        <v>444</v>
       </c>
     </row>
     <row r="88" spans="1:5" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A88" s="4" t="s">
-        <v>388</v>
+        <v>387</v>
       </c>
       <c r="B88" s="4" t="str">
         <f>VLOOKUP(A88,TableNames!$A$2:$B$12,2,FALSE)</f>
@@ -3667,15 +3667,15 @@
         <v>1</v>
       </c>
       <c r="D88" s="4" t="s">
-        <v>389</v>
+        <v>388</v>
       </c>
       <c r="E88" s="4" t="s">
-        <v>446</v>
+        <v>445</v>
       </c>
     </row>
     <row r="89" spans="1:5" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A89" s="4" t="s">
-        <v>388</v>
+        <v>387</v>
       </c>
       <c r="B89" s="4" t="str">
         <f>VLOOKUP(A89,TableNames!$A$2:$B$12,2,FALSE)</f>
@@ -3688,12 +3688,12 @@
         <v>319</v>
       </c>
       <c r="E89" s="4" t="s">
-        <v>405</v>
+        <v>404</v>
       </c>
     </row>
     <row r="90" spans="1:5" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A90" s="4" t="s">
-        <v>388</v>
+        <v>387</v>
       </c>
       <c r="B90" s="4" t="str">
         <f>VLOOKUP(A90,TableNames!$A$2:$B$12,2,FALSE)</f>
@@ -3706,12 +3706,12 @@
         <v>309</v>
       </c>
       <c r="E90" s="4" t="s">
-        <v>404</v>
+        <v>403</v>
       </c>
     </row>
     <row r="91" spans="1:5" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A91" s="4" t="s">
-        <v>388</v>
+        <v>387</v>
       </c>
       <c r="B91" s="4" t="str">
         <f>VLOOKUP(A91,TableNames!$A$2:$B$12,2,FALSE)</f>
@@ -3721,15 +3721,15 @@
         <v>4</v>
       </c>
       <c r="D91" s="4" t="s">
-        <v>390</v>
+        <v>389</v>
       </c>
       <c r="E91" s="4" t="s">
-        <v>447</v>
+        <v>446</v>
       </c>
     </row>
     <row r="92" spans="1:5" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A92" s="4" t="s">
-        <v>388</v>
+        <v>387</v>
       </c>
       <c r="B92" s="4" t="str">
         <f>VLOOKUP(A92,TableNames!$A$2:$B$12,2,FALSE)</f>
@@ -3739,15 +3739,15 @@
         <v>5</v>
       </c>
       <c r="D92" s="4" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
       <c r="E92" s="4" t="s">
-        <v>448</v>
+        <v>447</v>
       </c>
     </row>
     <row r="93" spans="1:5" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A93" s="4" t="s">
-        <v>388</v>
+        <v>387</v>
       </c>
       <c r="B93" s="4" t="str">
         <f>VLOOKUP(A93,TableNames!$A$2:$B$12,2,FALSE)</f>
@@ -3757,15 +3757,15 @@
         <v>6</v>
       </c>
       <c r="D93" s="4" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
       <c r="E93" s="4" t="s">
-        <v>449</v>
+        <v>448</v>
       </c>
     </row>
     <row r="94" spans="1:5" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A94" s="4" t="s">
-        <v>388</v>
+        <v>387</v>
       </c>
       <c r="B94" s="4" t="str">
         <f>VLOOKUP(A94,TableNames!$A$2:$B$12,2,FALSE)</f>
@@ -3775,15 +3775,15 @@
         <v>7</v>
       </c>
       <c r="D94" s="4" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
       <c r="E94" s="4" t="s">
-        <v>455</v>
+        <v>454</v>
       </c>
     </row>
     <row r="95" spans="1:5" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A95" s="4" t="s">
-        <v>394</v>
+        <v>393</v>
       </c>
       <c r="B95" s="4" t="str">
         <f>VLOOKUP(A95,TableNames!$A$2:$B$12,2,FALSE)</f>
@@ -3793,15 +3793,15 @@
         <v>1</v>
       </c>
       <c r="D95" s="4" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
       <c r="E95" s="4" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
     </row>
     <row r="96" spans="1:5" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A96" s="4" t="s">
-        <v>394</v>
+        <v>393</v>
       </c>
       <c r="B96" s="4" t="str">
         <f>VLOOKUP(A96,TableNames!$A$2:$B$12,2,FALSE)</f>
@@ -3814,12 +3814,12 @@
         <v>309</v>
       </c>
       <c r="E96" s="4" t="s">
-        <v>404</v>
+        <v>403</v>
       </c>
     </row>
     <row r="97" spans="1:5" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A97" s="4" t="s">
-        <v>394</v>
+        <v>393</v>
       </c>
       <c r="B97" s="4" t="str">
         <f>VLOOKUP(A97,TableNames!$A$2:$B$12,2,FALSE)</f>
@@ -3829,15 +3829,15 @@
         <v>3</v>
       </c>
       <c r="D97" s="4" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
       <c r="E97" s="4" t="s">
-        <v>473</v>
+        <v>472</v>
       </c>
     </row>
     <row r="98" spans="1:5" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A98" s="4" t="s">
-        <v>394</v>
+        <v>393</v>
       </c>
       <c r="B98" s="4" t="str">
         <f>VLOOKUP(A98,TableNames!$A$2:$B$12,2,FALSE)</f>
@@ -3847,7 +3847,7 @@
         <v>4</v>
       </c>
       <c r="D98" s="4" t="s">
-        <v>397</v>
+        <v>396</v>
       </c>
       <c r="E98" s="4" t="s">
         <v>280</v>
@@ -3855,7 +3855,7 @@
     </row>
     <row r="99" spans="1:5" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A99" s="4" t="s">
-        <v>394</v>
+        <v>393</v>
       </c>
       <c r="B99" s="4" t="str">
         <f>VLOOKUP(A99,TableNames!$A$2:$B$12,2,FALSE)</f>
@@ -3865,15 +3865,15 @@
         <v>5</v>
       </c>
       <c r="D99" s="4" t="s">
-        <v>398</v>
+        <v>397</v>
       </c>
       <c r="E99" s="4" t="s">
-        <v>450</v>
+        <v>449</v>
       </c>
     </row>
     <row r="100" spans="1:5" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A100" s="4" t="s">
-        <v>394</v>
+        <v>393</v>
       </c>
       <c r="B100" s="4" t="str">
         <f>VLOOKUP(A100,TableNames!$A$2:$B$12,2,FALSE)</f>
@@ -3883,15 +3883,15 @@
         <v>6</v>
       </c>
       <c r="D100" s="4" t="s">
-        <v>399</v>
+        <v>398</v>
       </c>
       <c r="E100" s="4" t="s">
-        <v>451</v>
+        <v>450</v>
       </c>
     </row>
     <row r="101" spans="1:5" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A101" s="4" t="s">
-        <v>394</v>
+        <v>393</v>
       </c>
       <c r="B101" s="4" t="str">
         <f>VLOOKUP(A101,TableNames!$A$2:$B$12,2,FALSE)</f>
@@ -3901,15 +3901,15 @@
         <v>7</v>
       </c>
       <c r="D101" s="4" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
       <c r="E101" s="4" t="s">
-        <v>452</v>
+        <v>451</v>
       </c>
     </row>
     <row r="102" spans="1:5" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A102" s="4" t="s">
-        <v>394</v>
+        <v>393</v>
       </c>
       <c r="B102" s="4" t="str">
         <f>VLOOKUP(A102,TableNames!$A$2:$B$12,2,FALSE)</f>
@@ -3919,15 +3919,15 @@
         <v>8</v>
       </c>
       <c r="D102" s="4" t="s">
-        <v>401</v>
+        <v>400</v>
       </c>
       <c r="E102" s="4" t="s">
-        <v>453</v>
+        <v>452</v>
       </c>
     </row>
     <row r="103" spans="1:5" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A103" s="4" t="s">
-        <v>394</v>
+        <v>393</v>
       </c>
       <c r="B103" s="4" t="str">
         <f>VLOOKUP(A103,TableNames!$A$2:$B$12,2,FALSE)</f>
@@ -3937,10 +3937,10 @@
         <v>9</v>
       </c>
       <c r="D103" s="4" t="s">
-        <v>402</v>
+        <v>401</v>
       </c>
       <c r="E103" s="4" t="s">
-        <v>454</v>
+        <v>453</v>
       </c>
     </row>
   </sheetData>
@@ -3953,8 +3953,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6EF1C1D3-3AE0-4822-BECE-5F11FDFA805B}">
   <dimension ref="A1:L256"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="D14" activePane="bottomRight" state="frozen"/>
+    <sheetView workbookViewId="0">
+      <pane xSplit="2" ySplit="1" topLeftCell="D187" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
       <selection pane="bottomRight" activeCell="G22" sqref="G22"/>
@@ -3978,25 +3978,25 @@
   <sheetData>
     <row r="1" spans="1:8" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="3" t="s">
-        <v>464</v>
+        <v>463</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>461</v>
+        <v>460</v>
       </c>
       <c r="C1" s="3" t="s">
         <v>193</v>
       </c>
       <c r="D1" s="3" t="s">
+        <v>461</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>464</v>
+      </c>
+      <c r="F1" s="7" t="s">
+        <v>465</v>
+      </c>
+      <c r="G1" s="2" t="s">
         <v>462</v>
-      </c>
-      <c r="E1" s="3" t="s">
-        <v>465</v>
-      </c>
-      <c r="F1" s="7" t="s">
-        <v>466</v>
-      </c>
-      <c r="G1" s="2" t="s">
-        <v>463</v>
       </c>
       <c r="H1" s="3" t="s">
         <v>194</v>
@@ -7759,13 +7759,13 @@
         <v>195</v>
       </c>
       <c r="D159" s="4" t="s">
+        <v>477</v>
+      </c>
+      <c r="E159" s="4" t="s">
+        <v>477</v>
+      </c>
+      <c r="F159" s="8" t="s">
         <v>478</v>
-      </c>
-      <c r="E159" s="4" t="s">
-        <v>478</v>
-      </c>
-      <c r="F159" s="8" t="s">
-        <v>479</v>
       </c>
     </row>
     <row r="160" spans="1:8" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
@@ -8761,13 +8761,13 @@
         <v>195</v>
       </c>
       <c r="D201" s="4" t="s">
+        <v>475</v>
+      </c>
+      <c r="E201" s="4" t="s">
+        <v>475</v>
+      </c>
+      <c r="F201" s="8" t="s">
         <v>476</v>
-      </c>
-      <c r="E201" s="4" t="s">
-        <v>476</v>
-      </c>
-      <c r="F201" s="8" t="s">
-        <v>477</v>
       </c>
       <c r="J201" s="5"/>
     </row>
@@ -9590,7 +9590,7 @@
         <v>261</v>
       </c>
       <c r="F236" s="8" t="s">
-        <v>491</v>
+        <v>490</v>
       </c>
       <c r="G236" s="5" t="s">
         <v>262</v>
@@ -10039,7 +10039,7 @@
         <v>46</v>
       </c>
       <c r="F253" s="9" t="s">
-        <v>490</v>
+        <v>489</v>
       </c>
       <c r="G253" s="5"/>
       <c r="J253" s="5"/>

</xml_diff>

<commit_message>
Changed ID colum names in meta data
</commit_message>
<xml_diff>
--- a/Development/Data/MetaData/MetaDataCCP.xlsx
+++ b/Development/Data/MetaData/MetaDataCCP.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Basti\ARBEIT Lokal\dsCCPhos\Development\Data\MetaData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{170431C0-9B27-42F0-986B-7C1B5A758EC9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{78123EA3-432A-4D42-A4E1-C9910236EA1F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="2" xr2:uid="{035133D3-9E9F-4CDB-BCDC-A149BB1E9383}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="16776" activeTab="1" xr2:uid="{035133D3-9E9F-4CDB-BCDC-A149BB1E9383}"/>
   </bookViews>
   <sheets>
     <sheet name="TableNames" sheetId="11" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1237" uniqueCount="494">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1237" uniqueCount="487">
   <si>
     <t>D</t>
   </si>
@@ -1022,9 +1022,6 @@
     <t>progress</t>
   </si>
   <si>
-    <t>progress-id</t>
-  </si>
-  <si>
     <t>untersuchungs-_befunddatum_im_verlauf</t>
   </si>
   <si>
@@ -1046,9 +1043,6 @@
     <t>histology</t>
   </si>
   <si>
-    <t>histology-id</t>
-  </si>
-  <si>
     <t>histologie_datum</t>
   </si>
   <si>
@@ -1067,9 +1061,6 @@
     <t>metastasis</t>
   </si>
   <si>
-    <t>metastasis-id</t>
-  </si>
-  <si>
     <t>datum_fernmetastasen</t>
   </si>
   <si>
@@ -1082,9 +1073,6 @@
     <t>tnm</t>
   </si>
   <si>
-    <t>tnm-id</t>
-  </si>
-  <si>
     <t>datum_der_tnm_dokumentation_datum_befund</t>
   </si>
   <si>
@@ -1124,9 +1112,6 @@
     <t>system-therapy</t>
   </si>
   <si>
-    <t>system-therapy-id</t>
-  </si>
-  <si>
     <t>intention_chemotherapie</t>
   </si>
   <si>
@@ -1163,9 +1148,6 @@
     <t>surgery</t>
   </si>
   <si>
-    <t>surgery-id</t>
-  </si>
-  <si>
     <t>ops-code</t>
   </si>
   <si>
@@ -1184,9 +1166,6 @@
     <t>radiation-therapy</t>
   </si>
   <si>
-    <t>radiation-therapy-id</t>
-  </si>
-  <si>
     <t>strahlentherapie_stellung_zu_operativer_therapie</t>
   </si>
   <si>
@@ -1220,9 +1199,6 @@
     <t>sample</t>
   </si>
   <si>
-    <t>sample-id</t>
-  </si>
-  <si>
     <t>entnahmedatum</t>
   </si>
   <si>
@@ -1518,6 +1494,9 @@
   </si>
   <si>
     <t>Table</t>
+  </si>
+  <si>
+    <t>_id</t>
   </si>
 </sst>
 </file>
@@ -1969,15 +1948,15 @@
   <sheetData>
     <row r="1" spans="1:2" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="3" t="s">
-        <v>455</v>
+        <v>447</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>462</v>
+        <v>454</v>
       </c>
     </row>
     <row r="2" spans="1:2" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="4" t="s">
-        <v>393</v>
+        <v>386</v>
       </c>
       <c r="B2" s="4" t="s">
         <v>277</v>
@@ -1993,7 +1972,7 @@
     </row>
     <row r="4" spans="1:2" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="4" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="B4" s="4" t="s">
         <v>169</v>
@@ -2001,7 +1980,7 @@
     </row>
     <row r="5" spans="1:2" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="4" t="s">
-        <v>342</v>
+        <v>340</v>
       </c>
       <c r="B5" s="4" t="s">
         <v>171</v>
@@ -2009,10 +1988,10 @@
     </row>
     <row r="6" spans="1:2" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="4" t="s">
-        <v>387</v>
+        <v>380</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>457</v>
+        <v>449</v>
       </c>
     </row>
     <row r="7" spans="1:2" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
@@ -2020,7 +1999,7 @@
         <v>308</v>
       </c>
       <c r="B7" s="4" t="s">
-        <v>459</v>
+        <v>451</v>
       </c>
     </row>
     <row r="8" spans="1:2" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
@@ -2033,15 +2012,15 @@
     </row>
     <row r="9" spans="1:2" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="4" t="s">
-        <v>381</v>
+        <v>375</v>
       </c>
       <c r="B9" s="4" t="s">
-        <v>456</v>
+        <v>448</v>
       </c>
     </row>
     <row r="10" spans="1:2" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" s="4" t="s">
-        <v>347</v>
+        <v>344</v>
       </c>
       <c r="B10" s="4" t="s">
         <v>170</v>
@@ -2049,7 +2028,7 @@
     </row>
     <row r="11" spans="1:2" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A11" s="4" t="s">
-        <v>374</v>
+        <v>369</v>
       </c>
       <c r="B11" s="4" t="s">
         <v>255</v>
@@ -2057,10 +2036,10 @@
     </row>
     <row r="12" spans="1:2" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A12" s="4" t="s">
-        <v>361</v>
+        <v>357</v>
       </c>
       <c r="B12" s="4" t="s">
-        <v>427</v>
+        <v>419</v>
       </c>
     </row>
   </sheetData>
@@ -2076,8 +2055,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CD8BF945-9186-40D3-A998-0B845CD0DDFC}">
   <dimension ref="A1:E103"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F4" sqref="F4"/>
+    <sheetView tabSelected="1" topLeftCell="A85" workbookViewId="0">
+      <selection activeCell="F92" sqref="F92"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="16.33203125" defaultRowHeight="25.2" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -2095,19 +2074,19 @@
   <sheetData>
     <row r="1" spans="1:5" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="3" t="s">
-        <v>455</v>
+        <v>447</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>462</v>
+        <v>454</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>402</v>
+        <v>394</v>
       </c>
       <c r="D1" s="3" t="s">
-        <v>458</v>
+        <v>450</v>
       </c>
       <c r="E1" s="3" t="s">
-        <v>465</v>
+        <v>457</v>
       </c>
     </row>
     <row r="2" spans="1:5" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
@@ -2122,10 +2101,10 @@
         <v>1</v>
       </c>
       <c r="D2" s="4" t="s">
-        <v>309</v>
+        <v>486</v>
       </c>
       <c r="E2" s="4" t="s">
-        <v>403</v>
+        <v>395</v>
       </c>
     </row>
     <row r="3" spans="1:5" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
@@ -2143,7 +2122,7 @@
         <v>310</v>
       </c>
       <c r="E3" s="4" t="s">
-        <v>405</v>
+        <v>397</v>
       </c>
     </row>
     <row r="4" spans="1:5" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
@@ -2161,7 +2140,7 @@
         <v>311</v>
       </c>
       <c r="E4" s="4" t="s">
-        <v>406</v>
+        <v>398</v>
       </c>
     </row>
     <row r="5" spans="1:5" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
@@ -2179,7 +2158,7 @@
         <v>312</v>
       </c>
       <c r="E5" s="4" t="s">
-        <v>407</v>
+        <v>399</v>
       </c>
     </row>
     <row r="6" spans="1:5" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
@@ -2197,7 +2176,7 @@
         <v>313</v>
       </c>
       <c r="E6" s="4" t="s">
-        <v>408</v>
+        <v>400</v>
       </c>
     </row>
     <row r="7" spans="1:5" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
@@ -2215,7 +2194,7 @@
         <v>314</v>
       </c>
       <c r="E7" s="4" t="s">
-        <v>468</v>
+        <v>460</v>
       </c>
     </row>
     <row r="8" spans="1:5" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
@@ -2251,7 +2230,7 @@
         <v>316</v>
       </c>
       <c r="E9" s="4" t="s">
-        <v>409</v>
+        <v>401</v>
       </c>
     </row>
     <row r="10" spans="1:5" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
@@ -2269,7 +2248,7 @@
         <v>317</v>
       </c>
       <c r="E10" s="4" t="s">
-        <v>410</v>
+        <v>402</v>
       </c>
     </row>
     <row r="11" spans="1:5" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
@@ -2284,10 +2263,10 @@
         <v>1</v>
       </c>
       <c r="D11" s="4" t="s">
-        <v>319</v>
+        <v>486</v>
       </c>
       <c r="E11" s="4" t="s">
-        <v>404</v>
+        <v>396</v>
       </c>
     </row>
     <row r="12" spans="1:5" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
@@ -2305,7 +2284,7 @@
         <v>309</v>
       </c>
       <c r="E12" s="4" t="s">
-        <v>403</v>
+        <v>395</v>
       </c>
     </row>
     <row r="13" spans="1:5" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
@@ -2323,7 +2302,7 @@
         <v>320</v>
       </c>
       <c r="E13" s="4" t="s">
-        <v>414</v>
+        <v>406</v>
       </c>
     </row>
     <row r="14" spans="1:5" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
@@ -2341,7 +2320,7 @@
         <v>321</v>
       </c>
       <c r="E14" s="4" t="s">
-        <v>479</v>
+        <v>471</v>
       </c>
     </row>
     <row r="15" spans="1:5" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
@@ -2359,7 +2338,7 @@
         <v>322</v>
       </c>
       <c r="E15" s="4" t="s">
-        <v>480</v>
+        <v>472</v>
       </c>
     </row>
     <row r="16" spans="1:5" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
@@ -2377,7 +2356,7 @@
         <v>323</v>
       </c>
       <c r="E16" s="4" t="s">
-        <v>411</v>
+        <v>403</v>
       </c>
     </row>
     <row r="17" spans="1:5" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
@@ -2395,7 +2374,7 @@
         <v>324</v>
       </c>
       <c r="E17" s="4" t="s">
-        <v>413</v>
+        <v>405</v>
       </c>
     </row>
     <row r="18" spans="1:5" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
@@ -2413,7 +2392,7 @@
         <v>325</v>
       </c>
       <c r="E18" s="4" t="s">
-        <v>412</v>
+        <v>404</v>
       </c>
     </row>
     <row r="19" spans="1:5" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
@@ -2446,10 +2425,10 @@
         <v>1</v>
       </c>
       <c r="D20" s="4" t="s">
-        <v>328</v>
+        <v>486</v>
       </c>
       <c r="E20" s="4" t="s">
-        <v>415</v>
+        <v>407</v>
       </c>
     </row>
     <row r="21" spans="1:5" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
@@ -2467,7 +2446,7 @@
         <v>319</v>
       </c>
       <c r="E21" s="4" t="s">
-        <v>404</v>
+        <v>396</v>
       </c>
     </row>
     <row r="22" spans="1:5" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
@@ -2485,7 +2464,7 @@
         <v>309</v>
       </c>
       <c r="E22" s="4" t="s">
-        <v>403</v>
+        <v>395</v>
       </c>
     </row>
     <row r="23" spans="1:5" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
@@ -2500,10 +2479,10 @@
         <v>4</v>
       </c>
       <c r="D23" s="4" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
       <c r="E23" s="4" t="s">
-        <v>478</v>
+        <v>470</v>
       </c>
     </row>
     <row r="24" spans="1:5" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
@@ -2518,10 +2497,10 @@
         <v>5</v>
       </c>
       <c r="D24" s="4" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="E24" s="4" t="s">
-        <v>469</v>
+        <v>461</v>
       </c>
     </row>
     <row r="25" spans="1:5" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
@@ -2536,10 +2515,10 @@
         <v>6</v>
       </c>
       <c r="D25" s="4" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
       <c r="E25" s="4" t="s">
-        <v>487</v>
+        <v>479</v>
       </c>
     </row>
     <row r="26" spans="1:5" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
@@ -2554,10 +2533,10 @@
         <v>7</v>
       </c>
       <c r="D26" s="4" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="E26" s="4" t="s">
-        <v>481</v>
+        <v>473</v>
       </c>
     </row>
     <row r="27" spans="1:5" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
@@ -2572,10 +2551,10 @@
         <v>8</v>
       </c>
       <c r="D27" s="4" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="E27" s="4" t="s">
-        <v>482</v>
+        <v>474</v>
       </c>
     </row>
     <row r="28" spans="1:5" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
@@ -2590,15 +2569,15 @@
         <v>9</v>
       </c>
       <c r="D28" s="4" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
       <c r="E28" s="4" t="s">
-        <v>483</v>
+        <v>475</v>
       </c>
     </row>
     <row r="29" spans="1:5" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A29" s="4" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="B29" s="4" t="str">
         <f>VLOOKUP(A29,TableNames!$A$2:$B$12,2,FALSE)</f>
@@ -2608,15 +2587,15 @@
         <v>1</v>
       </c>
       <c r="D29" s="4" t="s">
-        <v>336</v>
+        <v>486</v>
       </c>
       <c r="E29" s="4" t="s">
-        <v>416</v>
+        <v>408</v>
       </c>
     </row>
     <row r="30" spans="1:5" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A30" s="4" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="B30" s="4" t="str">
         <f>VLOOKUP(A30,TableNames!$A$2:$B$12,2,FALSE)</f>
@@ -2629,12 +2608,12 @@
         <v>319</v>
       </c>
       <c r="E30" s="4" t="s">
-        <v>404</v>
+        <v>396</v>
       </c>
     </row>
     <row r="31" spans="1:5" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A31" s="4" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="B31" s="4" t="str">
         <f>VLOOKUP(A31,TableNames!$A$2:$B$12,2,FALSE)</f>
@@ -2647,12 +2626,12 @@
         <v>309</v>
       </c>
       <c r="E31" s="4" t="s">
-        <v>403</v>
+        <v>395</v>
       </c>
     </row>
     <row r="32" spans="1:5" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A32" s="4" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="B32" s="4" t="str">
         <f>VLOOKUP(A32,TableNames!$A$2:$B$12,2,FALSE)</f>
@@ -2662,15 +2641,15 @@
         <v>4</v>
       </c>
       <c r="D32" s="4" t="s">
-        <v>337</v>
+        <v>335</v>
       </c>
       <c r="E32" s="4" t="s">
-        <v>470</v>
+        <v>462</v>
       </c>
     </row>
     <row r="33" spans="1:5" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A33" s="4" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="B33" s="4" t="str">
         <f>VLOOKUP(A33,TableNames!$A$2:$B$12,2,FALSE)</f>
@@ -2680,15 +2659,15 @@
         <v>5</v>
       </c>
       <c r="D33" s="4" t="s">
-        <v>338</v>
+        <v>336</v>
       </c>
       <c r="E33" s="4" t="s">
-        <v>420</v>
+        <v>412</v>
       </c>
     </row>
     <row r="34" spans="1:5" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A34" s="4" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="B34" s="4" t="str">
         <f>VLOOKUP(A34,TableNames!$A$2:$B$12,2,FALSE)</f>
@@ -2698,15 +2677,15 @@
         <v>6</v>
       </c>
       <c r="D34" s="4" t="s">
-        <v>339</v>
+        <v>337</v>
       </c>
       <c r="E34" s="4" t="s">
-        <v>421</v>
+        <v>413</v>
       </c>
     </row>
     <row r="35" spans="1:5" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A35" s="4" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="B35" s="4" t="str">
         <f>VLOOKUP(A35,TableNames!$A$2:$B$12,2,FALSE)</f>
@@ -2716,15 +2695,15 @@
         <v>7</v>
       </c>
       <c r="D35" s="4" t="s">
-        <v>340</v>
+        <v>338</v>
       </c>
       <c r="E35" s="4" t="s">
-        <v>490</v>
+        <v>482</v>
       </c>
     </row>
     <row r="36" spans="1:5" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A36" s="4" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="B36" s="4" t="str">
         <f>VLOOKUP(A36,TableNames!$A$2:$B$12,2,FALSE)</f>
@@ -2734,7 +2713,7 @@
         <v>8</v>
       </c>
       <c r="D36" s="4" t="s">
-        <v>341</v>
+        <v>339</v>
       </c>
       <c r="E36" s="4" t="s">
         <v>11</v>
@@ -2742,7 +2721,7 @@
     </row>
     <row r="37" spans="1:5" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A37" s="4" t="s">
-        <v>342</v>
+        <v>340</v>
       </c>
       <c r="B37" s="4" t="str">
         <f>VLOOKUP(A37,TableNames!$A$2:$B$12,2,FALSE)</f>
@@ -2752,15 +2731,15 @@
         <v>1</v>
       </c>
       <c r="D37" s="4" t="s">
-        <v>343</v>
+        <v>486</v>
       </c>
       <c r="E37" s="4" t="s">
-        <v>417</v>
+        <v>409</v>
       </c>
     </row>
     <row r="38" spans="1:5" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A38" s="4" t="s">
-        <v>342</v>
+        <v>340</v>
       </c>
       <c r="B38" s="4" t="str">
         <f>VLOOKUP(A38,TableNames!$A$2:$B$12,2,FALSE)</f>
@@ -2773,12 +2752,12 @@
         <v>319</v>
       </c>
       <c r="E38" s="4" t="s">
-        <v>404</v>
+        <v>396</v>
       </c>
     </row>
     <row r="39" spans="1:5" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A39" s="4" t="s">
-        <v>342</v>
+        <v>340</v>
       </c>
       <c r="B39" s="4" t="str">
         <f>VLOOKUP(A39,TableNames!$A$2:$B$12,2,FALSE)</f>
@@ -2791,12 +2770,12 @@
         <v>309</v>
       </c>
       <c r="E39" s="4" t="s">
-        <v>403</v>
+        <v>395</v>
       </c>
     </row>
     <row r="40" spans="1:5" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A40" s="4" t="s">
-        <v>342</v>
+        <v>340</v>
       </c>
       <c r="B40" s="4" t="str">
         <f>VLOOKUP(A40,TableNames!$A$2:$B$12,2,FALSE)</f>
@@ -2806,15 +2785,15 @@
         <v>4</v>
       </c>
       <c r="D40" s="4" t="s">
-        <v>344</v>
+        <v>341</v>
       </c>
       <c r="E40" s="4" t="s">
-        <v>467</v>
+        <v>459</v>
       </c>
     </row>
     <row r="41" spans="1:5" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A41" s="4" t="s">
-        <v>342</v>
+        <v>340</v>
       </c>
       <c r="B41" s="4" t="str">
         <f>VLOOKUP(A41,TableNames!$A$2:$B$12,2,FALSE)</f>
@@ -2824,15 +2803,15 @@
         <v>5</v>
       </c>
       <c r="D41" s="4" t="s">
-        <v>345</v>
+        <v>342</v>
       </c>
       <c r="E41" s="4" t="s">
-        <v>484</v>
+        <v>476</v>
       </c>
     </row>
     <row r="42" spans="1:5" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A42" s="4" t="s">
-        <v>342</v>
+        <v>340</v>
       </c>
       <c r="B42" s="4" t="str">
         <f>VLOOKUP(A42,TableNames!$A$2:$B$12,2,FALSE)</f>
@@ -2842,15 +2821,15 @@
         <v>6</v>
       </c>
       <c r="D42" s="4" t="s">
-        <v>346</v>
+        <v>343</v>
       </c>
       <c r="E42" s="4" t="s">
-        <v>485</v>
+        <v>477</v>
       </c>
     </row>
     <row r="43" spans="1:5" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A43" s="4" t="s">
-        <v>347</v>
+        <v>344</v>
       </c>
       <c r="B43" s="4" t="str">
         <f>VLOOKUP(A43,TableNames!$A$2:$B$12,2,FALSE)</f>
@@ -2860,15 +2839,15 @@
         <v>1</v>
       </c>
       <c r="D43" s="4" t="s">
-        <v>348</v>
+        <v>486</v>
       </c>
       <c r="E43" s="4" t="s">
-        <v>422</v>
+        <v>414</v>
       </c>
     </row>
     <row r="44" spans="1:5" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A44" s="4" t="s">
-        <v>347</v>
+        <v>344</v>
       </c>
       <c r="B44" s="4" t="str">
         <f>VLOOKUP(A44,TableNames!$A$2:$B$12,2,FALSE)</f>
@@ -2881,12 +2860,12 @@
         <v>319</v>
       </c>
       <c r="E44" s="4" t="s">
-        <v>404</v>
+        <v>396</v>
       </c>
     </row>
     <row r="45" spans="1:5" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A45" s="4" t="s">
-        <v>347</v>
+        <v>344</v>
       </c>
       <c r="B45" s="4" t="str">
         <f>VLOOKUP(A45,TableNames!$A$2:$B$12,2,FALSE)</f>
@@ -2899,12 +2878,12 @@
         <v>309</v>
       </c>
       <c r="E45" s="4" t="s">
-        <v>403</v>
+        <v>395</v>
       </c>
     </row>
     <row r="46" spans="1:5" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A46" s="4" t="s">
-        <v>347</v>
+        <v>344</v>
       </c>
       <c r="B46" s="4" t="str">
         <f>VLOOKUP(A46,TableNames!$A$2:$B$12,2,FALSE)</f>
@@ -2914,15 +2893,15 @@
         <v>4</v>
       </c>
       <c r="D46" s="4" t="s">
-        <v>349</v>
+        <v>345</v>
       </c>
       <c r="E46" s="4" t="s">
-        <v>486</v>
+        <v>478</v>
       </c>
     </row>
     <row r="47" spans="1:5" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A47" s="4" t="s">
-        <v>347</v>
+        <v>344</v>
       </c>
       <c r="B47" s="4" t="str">
         <f>VLOOKUP(A47,TableNames!$A$2:$B$12,2,FALSE)</f>
@@ -2932,7 +2911,7 @@
         <v>5</v>
       </c>
       <c r="D47" s="4" t="s">
-        <v>350</v>
+        <v>346</v>
       </c>
       <c r="E47" s="4" t="s">
         <v>28</v>
@@ -2940,7 +2919,7 @@
     </row>
     <row r="48" spans="1:5" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A48" s="4" t="s">
-        <v>347</v>
+        <v>344</v>
       </c>
       <c r="B48" s="4" t="str">
         <f>VLOOKUP(A48,TableNames!$A$2:$B$12,2,FALSE)</f>
@@ -2950,7 +2929,7 @@
         <v>6</v>
       </c>
       <c r="D48" s="4" t="s">
-        <v>351</v>
+        <v>347</v>
       </c>
       <c r="E48" s="4" t="s">
         <v>29</v>
@@ -2958,7 +2937,7 @@
     </row>
     <row r="49" spans="1:5" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A49" s="4" t="s">
-        <v>347</v>
+        <v>344</v>
       </c>
       <c r="B49" s="4" t="str">
         <f>VLOOKUP(A49,TableNames!$A$2:$B$12,2,FALSE)</f>
@@ -2968,7 +2947,7 @@
         <v>7</v>
       </c>
       <c r="D49" s="4" t="s">
-        <v>352</v>
+        <v>348</v>
       </c>
       <c r="E49" s="4" t="s">
         <v>30</v>
@@ -2976,7 +2955,7 @@
     </row>
     <row r="50" spans="1:5" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A50" s="4" t="s">
-        <v>347</v>
+        <v>344</v>
       </c>
       <c r="B50" s="4" t="str">
         <f>VLOOKUP(A50,TableNames!$A$2:$B$12,2,FALSE)</f>
@@ -2986,7 +2965,7 @@
         <v>8</v>
       </c>
       <c r="D50" s="4" t="s">
-        <v>353</v>
+        <v>349</v>
       </c>
       <c r="E50" s="4" t="s">
         <v>31</v>
@@ -2994,7 +2973,7 @@
     </row>
     <row r="51" spans="1:5" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A51" s="4" t="s">
-        <v>347</v>
+        <v>344</v>
       </c>
       <c r="B51" s="4" t="str">
         <f>VLOOKUP(A51,TableNames!$A$2:$B$12,2,FALSE)</f>
@@ -3004,7 +2983,7 @@
         <v>9</v>
       </c>
       <c r="D51" s="4" t="s">
-        <v>354</v>
+        <v>350</v>
       </c>
       <c r="E51" s="4" t="s">
         <v>32</v>
@@ -3012,7 +2991,7 @@
     </row>
     <row r="52" spans="1:5" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A52" s="4" t="s">
-        <v>347</v>
+        <v>344</v>
       </c>
       <c r="B52" s="4" t="str">
         <f>VLOOKUP(A52,TableNames!$A$2:$B$12,2,FALSE)</f>
@@ -3022,7 +3001,7 @@
         <v>10</v>
       </c>
       <c r="D52" s="4" t="s">
-        <v>355</v>
+        <v>351</v>
       </c>
       <c r="E52" s="4" t="s">
         <v>33</v>
@@ -3030,7 +3009,7 @@
     </row>
     <row r="53" spans="1:5" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A53" s="4" t="s">
-        <v>347</v>
+        <v>344</v>
       </c>
       <c r="B53" s="4" t="str">
         <f>VLOOKUP(A53,TableNames!$A$2:$B$12,2,FALSE)</f>
@@ -3040,7 +3019,7 @@
         <v>11</v>
       </c>
       <c r="D53" s="4" t="s">
-        <v>356</v>
+        <v>352</v>
       </c>
       <c r="E53" s="4" t="s">
         <v>34</v>
@@ -3048,7 +3027,7 @@
     </row>
     <row r="54" spans="1:5" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A54" s="4" t="s">
-        <v>347</v>
+        <v>344</v>
       </c>
       <c r="B54" s="4" t="str">
         <f>VLOOKUP(A54,TableNames!$A$2:$B$12,2,FALSE)</f>
@@ -3058,15 +3037,15 @@
         <v>12</v>
       </c>
       <c r="D54" s="4" t="s">
-        <v>357</v>
+        <v>353</v>
       </c>
       <c r="E54" s="4" t="s">
-        <v>473</v>
+        <v>465</v>
       </c>
     </row>
     <row r="55" spans="1:5" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A55" s="4" t="s">
-        <v>347</v>
+        <v>344</v>
       </c>
       <c r="B55" s="4" t="str">
         <f>VLOOKUP(A55,TableNames!$A$2:$B$12,2,FALSE)</f>
@@ -3076,15 +3055,15 @@
         <v>13</v>
       </c>
       <c r="D55" s="4" t="s">
-        <v>358</v>
+        <v>354</v>
       </c>
       <c r="E55" s="4" t="s">
-        <v>423</v>
+        <v>415</v>
       </c>
     </row>
     <row r="56" spans="1:5" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A56" s="4" t="s">
-        <v>347</v>
+        <v>344</v>
       </c>
       <c r="B56" s="4" t="str">
         <f>VLOOKUP(A56,TableNames!$A$2:$B$12,2,FALSE)</f>
@@ -3094,15 +3073,15 @@
         <v>14</v>
       </c>
       <c r="D56" s="4" t="s">
-        <v>359</v>
+        <v>355</v>
       </c>
       <c r="E56" s="4" t="s">
-        <v>424</v>
+        <v>416</v>
       </c>
     </row>
     <row r="57" spans="1:5" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A57" s="4" t="s">
-        <v>347</v>
+        <v>344</v>
       </c>
       <c r="B57" s="4" t="str">
         <f>VLOOKUP(A57,TableNames!$A$2:$B$12,2,FALSE)</f>
@@ -3112,15 +3091,15 @@
         <v>15</v>
       </c>
       <c r="D57" s="4" t="s">
-        <v>360</v>
+        <v>356</v>
       </c>
       <c r="E57" s="4" t="s">
-        <v>425</v>
+        <v>417</v>
       </c>
     </row>
     <row r="58" spans="1:5" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A58" s="4" t="s">
-        <v>361</v>
+        <v>357</v>
       </c>
       <c r="B58" s="4" t="str">
         <f>VLOOKUP(A58,TableNames!$A$2:$B$12,2,FALSE)</f>
@@ -3130,15 +3109,15 @@
         <v>1</v>
       </c>
       <c r="D58" s="4" t="s">
-        <v>362</v>
+        <v>486</v>
       </c>
       <c r="E58" s="4" t="s">
-        <v>426</v>
+        <v>418</v>
       </c>
     </row>
     <row r="59" spans="1:5" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A59" s="4" t="s">
-        <v>361</v>
+        <v>357</v>
       </c>
       <c r="B59" s="4" t="str">
         <f>VLOOKUP(A59,TableNames!$A$2:$B$12,2,FALSE)</f>
@@ -3151,12 +3130,12 @@
         <v>319</v>
       </c>
       <c r="E59" s="4" t="s">
-        <v>404</v>
+        <v>396</v>
       </c>
     </row>
     <row r="60" spans="1:5" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A60" s="4" t="s">
-        <v>361</v>
+        <v>357</v>
       </c>
       <c r="B60" s="4" t="str">
         <f>VLOOKUP(A60,TableNames!$A$2:$B$12,2,FALSE)</f>
@@ -3169,12 +3148,12 @@
         <v>309</v>
       </c>
       <c r="E60" s="4" t="s">
-        <v>403</v>
+        <v>395</v>
       </c>
     </row>
     <row r="61" spans="1:5" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A61" s="4" t="s">
-        <v>361</v>
+        <v>357</v>
       </c>
       <c r="B61" s="4" t="str">
         <f>VLOOKUP(A61,TableNames!$A$2:$B$12,2,FALSE)</f>
@@ -3184,15 +3163,15 @@
         <v>4</v>
       </c>
       <c r="D61" s="4" t="s">
-        <v>491</v>
+        <v>483</v>
       </c>
       <c r="E61" s="4" t="s">
-        <v>439</v>
+        <v>431</v>
       </c>
     </row>
     <row r="62" spans="1:5" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A62" s="4" t="s">
-        <v>361</v>
+        <v>357</v>
       </c>
       <c r="B62" s="4" t="str">
         <f>VLOOKUP(A62,TableNames!$A$2:$B$12,2,FALSE)</f>
@@ -3202,15 +3181,15 @@
         <v>5</v>
       </c>
       <c r="D62" s="4" t="s">
-        <v>363</v>
+        <v>358</v>
       </c>
       <c r="E62" s="4" t="s">
-        <v>472</v>
+        <v>464</v>
       </c>
     </row>
     <row r="63" spans="1:5" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A63" s="4" t="s">
-        <v>361</v>
+        <v>357</v>
       </c>
       <c r="B63" s="4" t="str">
         <f>VLOOKUP(A63,TableNames!$A$2:$B$12,2,FALSE)</f>
@@ -3220,15 +3199,15 @@
         <v>6</v>
       </c>
       <c r="D63" s="4" t="s">
-        <v>364</v>
+        <v>359</v>
       </c>
       <c r="E63" s="4" t="s">
-        <v>428</v>
+        <v>420</v>
       </c>
     </row>
     <row r="64" spans="1:5" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A64" s="4" t="s">
-        <v>361</v>
+        <v>357</v>
       </c>
       <c r="B64" s="4" t="str">
         <f>VLOOKUP(A64,TableNames!$A$2:$B$12,2,FALSE)</f>
@@ -3238,15 +3217,15 @@
         <v>7</v>
       </c>
       <c r="D64" s="4" t="s">
-        <v>365</v>
+        <v>360</v>
       </c>
       <c r="E64" s="4" t="s">
-        <v>429</v>
+        <v>421</v>
       </c>
     </row>
     <row r="65" spans="1:5" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A65" s="4" t="s">
-        <v>361</v>
+        <v>357</v>
       </c>
       <c r="B65" s="4" t="str">
         <f>VLOOKUP(A65,TableNames!$A$2:$B$12,2,FALSE)</f>
@@ -3256,15 +3235,15 @@
         <v>8</v>
       </c>
       <c r="D65" s="4" t="s">
-        <v>366</v>
+        <v>361</v>
       </c>
       <c r="E65" s="4" t="s">
-        <v>430</v>
+        <v>422</v>
       </c>
     </row>
     <row r="66" spans="1:5" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A66" s="4" t="s">
-        <v>361</v>
+        <v>357</v>
       </c>
       <c r="B66" s="4" t="str">
         <f>VLOOKUP(A66,TableNames!$A$2:$B$12,2,FALSE)</f>
@@ -3274,15 +3253,15 @@
         <v>9</v>
       </c>
       <c r="D66" s="4" t="s">
-        <v>367</v>
+        <v>362</v>
       </c>
       <c r="E66" s="4" t="s">
-        <v>431</v>
+        <v>423</v>
       </c>
     </row>
     <row r="67" spans="1:5" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A67" s="4" t="s">
-        <v>361</v>
+        <v>357</v>
       </c>
       <c r="B67" s="4" t="str">
         <f>VLOOKUP(A67,TableNames!$A$2:$B$12,2,FALSE)</f>
@@ -3292,15 +3271,15 @@
         <v>10</v>
       </c>
       <c r="D67" s="4" t="s">
-        <v>368</v>
+        <v>363</v>
       </c>
       <c r="E67" s="4" t="s">
-        <v>432</v>
+        <v>424</v>
       </c>
     </row>
     <row r="68" spans="1:5" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A68" s="4" t="s">
-        <v>361</v>
+        <v>357</v>
       </c>
       <c r="B68" s="4" t="str">
         <f>VLOOKUP(A68,TableNames!$A$2:$B$12,2,FALSE)</f>
@@ -3310,15 +3289,15 @@
         <v>11</v>
       </c>
       <c r="D68" s="4" t="s">
-        <v>369</v>
+        <v>364</v>
       </c>
       <c r="E68" s="4" t="s">
-        <v>433</v>
+        <v>425</v>
       </c>
     </row>
     <row r="69" spans="1:5" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A69" s="4" t="s">
-        <v>361</v>
+        <v>357</v>
       </c>
       <c r="B69" s="4" t="str">
         <f>VLOOKUP(A69,TableNames!$A$2:$B$12,2,FALSE)</f>
@@ -3328,15 +3307,15 @@
         <v>12</v>
       </c>
       <c r="D69" s="4" t="s">
-        <v>370</v>
+        <v>365</v>
       </c>
       <c r="E69" s="4" t="s">
-        <v>466</v>
+        <v>458</v>
       </c>
     </row>
     <row r="70" spans="1:5" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A70" s="4" t="s">
-        <v>361</v>
+        <v>357</v>
       </c>
       <c r="B70" s="4" t="str">
         <f>VLOOKUP(A70,TableNames!$A$2:$B$12,2,FALSE)</f>
@@ -3346,15 +3325,15 @@
         <v>13</v>
       </c>
       <c r="D70" s="4" t="s">
-        <v>371</v>
+        <v>366</v>
       </c>
       <c r="E70" s="4" t="s">
-        <v>434</v>
+        <v>426</v>
       </c>
     </row>
     <row r="71" spans="1:5" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A71" s="4" t="s">
-        <v>361</v>
+        <v>357</v>
       </c>
       <c r="B71" s="4" t="str">
         <f>VLOOKUP(A71,TableNames!$A$2:$B$12,2,FALSE)</f>
@@ -3364,15 +3343,15 @@
         <v>14</v>
       </c>
       <c r="D71" s="4" t="s">
-        <v>372</v>
+        <v>367</v>
       </c>
       <c r="E71" s="4" t="s">
-        <v>435</v>
+        <v>427</v>
       </c>
     </row>
     <row r="72" spans="1:5" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A72" s="4" t="s">
-        <v>361</v>
+        <v>357</v>
       </c>
       <c r="B72" s="4" t="str">
         <f>VLOOKUP(A72,TableNames!$A$2:$B$12,2,FALSE)</f>
@@ -3382,15 +3361,15 @@
         <v>15</v>
       </c>
       <c r="D72" s="4" t="s">
-        <v>373</v>
+        <v>368</v>
       </c>
       <c r="E72" s="4" t="s">
-        <v>436</v>
+        <v>428</v>
       </c>
     </row>
     <row r="73" spans="1:5" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A73" s="4" t="s">
-        <v>374</v>
+        <v>369</v>
       </c>
       <c r="B73" s="4" t="str">
         <f>VLOOKUP(A73,TableNames!$A$2:$B$12,2,FALSE)</f>
@@ -3400,15 +3379,15 @@
         <v>1</v>
       </c>
       <c r="D73" s="4" t="s">
-        <v>375</v>
+        <v>486</v>
       </c>
       <c r="E73" s="4" t="s">
-        <v>418</v>
+        <v>410</v>
       </c>
     </row>
     <row r="74" spans="1:5" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A74" s="4" t="s">
-        <v>374</v>
+        <v>369</v>
       </c>
       <c r="B74" s="4" t="str">
         <f>VLOOKUP(A74,TableNames!$A$2:$B$12,2,FALSE)</f>
@@ -3421,12 +3400,12 @@
         <v>319</v>
       </c>
       <c r="E74" s="4" t="s">
-        <v>404</v>
+        <v>396</v>
       </c>
     </row>
     <row r="75" spans="1:5" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A75" s="4" t="s">
-        <v>374</v>
+        <v>369</v>
       </c>
       <c r="B75" s="4" t="str">
         <f>VLOOKUP(A75,TableNames!$A$2:$B$12,2,FALSE)</f>
@@ -3439,12 +3418,12 @@
         <v>309</v>
       </c>
       <c r="E75" s="4" t="s">
-        <v>403</v>
+        <v>395</v>
       </c>
     </row>
     <row r="76" spans="1:5" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A76" s="4" t="s">
-        <v>374</v>
+        <v>369</v>
       </c>
       <c r="B76" s="4" t="str">
         <f>VLOOKUP(A76,TableNames!$A$2:$B$12,2,FALSE)</f>
@@ -3454,15 +3433,15 @@
         <v>4</v>
       </c>
       <c r="D76" s="4" t="s">
-        <v>376</v>
+        <v>370</v>
       </c>
       <c r="E76" s="4" t="s">
-        <v>437</v>
+        <v>429</v>
       </c>
     </row>
     <row r="77" spans="1:5" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A77" s="4" t="s">
-        <v>374</v>
+        <v>369</v>
       </c>
       <c r="B77" s="4" t="str">
         <f>VLOOKUP(A77,TableNames!$A$2:$B$12,2,FALSE)</f>
@@ -3472,15 +3451,15 @@
         <v>5</v>
       </c>
       <c r="D77" s="4" t="s">
-        <v>377</v>
+        <v>371</v>
       </c>
       <c r="E77" s="4" t="s">
-        <v>438</v>
+        <v>430</v>
       </c>
     </row>
     <row r="78" spans="1:5" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A78" s="4" t="s">
-        <v>374</v>
+        <v>369</v>
       </c>
       <c r="B78" s="4" t="str">
         <f>VLOOKUP(A78,TableNames!$A$2:$B$12,2,FALSE)</f>
@@ -3490,7 +3469,7 @@
         <v>6</v>
       </c>
       <c r="D78" s="4" t="s">
-        <v>378</v>
+        <v>372</v>
       </c>
       <c r="E78" s="4" t="s">
         <v>173</v>
@@ -3498,7 +3477,7 @@
     </row>
     <row r="79" spans="1:5" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A79" s="4" t="s">
-        <v>374</v>
+        <v>369</v>
       </c>
       <c r="B79" s="4" t="str">
         <f>VLOOKUP(A79,TableNames!$A$2:$B$12,2,FALSE)</f>
@@ -3508,7 +3487,7 @@
         <v>7</v>
       </c>
       <c r="D79" s="4" t="s">
-        <v>379</v>
+        <v>373</v>
       </c>
       <c r="E79" s="4" t="s">
         <v>256</v>
@@ -3516,7 +3495,7 @@
     </row>
     <row r="80" spans="1:5" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A80" s="4" t="s">
-        <v>374</v>
+        <v>369</v>
       </c>
       <c r="B80" s="4" t="str">
         <f>VLOOKUP(A80,TableNames!$A$2:$B$12,2,FALSE)</f>
@@ -3526,7 +3505,7 @@
         <v>8</v>
       </c>
       <c r="D80" s="4" t="s">
-        <v>380</v>
+        <v>374</v>
       </c>
       <c r="E80" s="4" t="s">
         <v>274</v>
@@ -3534,7 +3513,7 @@
     </row>
     <row r="81" spans="1:5" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A81" s="4" t="s">
-        <v>381</v>
+        <v>375</v>
       </c>
       <c r="B81" s="4" t="str">
         <f>VLOOKUP(A81,TableNames!$A$2:$B$12,2,FALSE)</f>
@@ -3544,15 +3523,15 @@
         <v>1</v>
       </c>
       <c r="D81" s="4" t="s">
-        <v>382</v>
+        <v>486</v>
       </c>
       <c r="E81" s="4" t="s">
-        <v>440</v>
+        <v>432</v>
       </c>
     </row>
     <row r="82" spans="1:5" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A82" s="4" t="s">
-        <v>381</v>
+        <v>375</v>
       </c>
       <c r="B82" s="4" t="str">
         <f>VLOOKUP(A82,TableNames!$A$2:$B$12,2,FALSE)</f>
@@ -3565,12 +3544,12 @@
         <v>319</v>
       </c>
       <c r="E82" s="4" t="s">
-        <v>404</v>
+        <v>396</v>
       </c>
     </row>
     <row r="83" spans="1:5" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A83" s="4" t="s">
-        <v>381</v>
+        <v>375</v>
       </c>
       <c r="B83" s="4" t="str">
         <f>VLOOKUP(A83,TableNames!$A$2:$B$12,2,FALSE)</f>
@@ -3583,12 +3562,12 @@
         <v>309</v>
       </c>
       <c r="E83" s="4" t="s">
-        <v>403</v>
+        <v>395</v>
       </c>
     </row>
     <row r="84" spans="1:5" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A84" s="4" t="s">
-        <v>381</v>
+        <v>375</v>
       </c>
       <c r="B84" s="4" t="str">
         <f>VLOOKUP(A84,TableNames!$A$2:$B$12,2,FALSE)</f>
@@ -3598,15 +3577,15 @@
         <v>4</v>
       </c>
       <c r="D84" s="4" t="s">
-        <v>383</v>
+        <v>376</v>
       </c>
       <c r="E84" s="4" t="s">
-        <v>441</v>
+        <v>433</v>
       </c>
     </row>
     <row r="85" spans="1:5" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A85" s="4" t="s">
-        <v>381</v>
+        <v>375</v>
       </c>
       <c r="B85" s="4" t="str">
         <f>VLOOKUP(A85,TableNames!$A$2:$B$12,2,FALSE)</f>
@@ -3616,15 +3595,15 @@
         <v>5</v>
       </c>
       <c r="D85" s="4" t="s">
-        <v>384</v>
+        <v>377</v>
       </c>
       <c r="E85" s="4" t="s">
-        <v>442</v>
+        <v>434</v>
       </c>
     </row>
     <row r="86" spans="1:5" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A86" s="4" t="s">
-        <v>381</v>
+        <v>375</v>
       </c>
       <c r="B86" s="4" t="str">
         <f>VLOOKUP(A86,TableNames!$A$2:$B$12,2,FALSE)</f>
@@ -3634,15 +3613,15 @@
         <v>6</v>
       </c>
       <c r="D86" s="4" t="s">
-        <v>385</v>
+        <v>378</v>
       </c>
       <c r="E86" s="4" t="s">
-        <v>443</v>
+        <v>435</v>
       </c>
     </row>
     <row r="87" spans="1:5" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A87" s="4" t="s">
-        <v>381</v>
+        <v>375</v>
       </c>
       <c r="B87" s="4" t="str">
         <f>VLOOKUP(A87,TableNames!$A$2:$B$12,2,FALSE)</f>
@@ -3652,15 +3631,15 @@
         <v>7</v>
       </c>
       <c r="D87" s="4" t="s">
-        <v>386</v>
+        <v>379</v>
       </c>
       <c r="E87" s="4" t="s">
-        <v>444</v>
+        <v>436</v>
       </c>
     </row>
     <row r="88" spans="1:5" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A88" s="4" t="s">
-        <v>387</v>
+        <v>380</v>
       </c>
       <c r="B88" s="4" t="str">
         <f>VLOOKUP(A88,TableNames!$A$2:$B$12,2,FALSE)</f>
@@ -3670,15 +3649,15 @@
         <v>1</v>
       </c>
       <c r="D88" s="4" t="s">
-        <v>388</v>
+        <v>381</v>
       </c>
       <c r="E88" s="4" t="s">
-        <v>445</v>
+        <v>437</v>
       </c>
     </row>
     <row r="89" spans="1:5" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A89" s="4" t="s">
-        <v>387</v>
+        <v>380</v>
       </c>
       <c r="B89" s="4" t="str">
         <f>VLOOKUP(A89,TableNames!$A$2:$B$12,2,FALSE)</f>
@@ -3691,12 +3670,12 @@
         <v>319</v>
       </c>
       <c r="E89" s="4" t="s">
-        <v>404</v>
+        <v>396</v>
       </c>
     </row>
     <row r="90" spans="1:5" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A90" s="4" t="s">
-        <v>387</v>
+        <v>380</v>
       </c>
       <c r="B90" s="4" t="str">
         <f>VLOOKUP(A90,TableNames!$A$2:$B$12,2,FALSE)</f>
@@ -3709,12 +3688,12 @@
         <v>309</v>
       </c>
       <c r="E90" s="4" t="s">
-        <v>403</v>
+        <v>395</v>
       </c>
     </row>
     <row r="91" spans="1:5" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A91" s="4" t="s">
-        <v>387</v>
+        <v>380</v>
       </c>
       <c r="B91" s="4" t="str">
         <f>VLOOKUP(A91,TableNames!$A$2:$B$12,2,FALSE)</f>
@@ -3724,15 +3703,15 @@
         <v>4</v>
       </c>
       <c r="D91" s="4" t="s">
-        <v>389</v>
+        <v>382</v>
       </c>
       <c r="E91" s="4" t="s">
-        <v>446</v>
+        <v>438</v>
       </c>
     </row>
     <row r="92" spans="1:5" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A92" s="4" t="s">
-        <v>387</v>
+        <v>380</v>
       </c>
       <c r="B92" s="4" t="str">
         <f>VLOOKUP(A92,TableNames!$A$2:$B$12,2,FALSE)</f>
@@ -3742,15 +3721,15 @@
         <v>5</v>
       </c>
       <c r="D92" s="4" t="s">
-        <v>390</v>
+        <v>383</v>
       </c>
       <c r="E92" s="4" t="s">
-        <v>447</v>
+        <v>439</v>
       </c>
     </row>
     <row r="93" spans="1:5" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A93" s="4" t="s">
-        <v>387</v>
+        <v>380</v>
       </c>
       <c r="B93" s="4" t="str">
         <f>VLOOKUP(A93,TableNames!$A$2:$B$12,2,FALSE)</f>
@@ -3760,15 +3739,15 @@
         <v>6</v>
       </c>
       <c r="D93" s="4" t="s">
-        <v>391</v>
+        <v>384</v>
       </c>
       <c r="E93" s="4" t="s">
-        <v>448</v>
+        <v>440</v>
       </c>
     </row>
     <row r="94" spans="1:5" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A94" s="4" t="s">
-        <v>387</v>
+        <v>380</v>
       </c>
       <c r="B94" s="4" t="str">
         <f>VLOOKUP(A94,TableNames!$A$2:$B$12,2,FALSE)</f>
@@ -3778,15 +3757,15 @@
         <v>7</v>
       </c>
       <c r="D94" s="4" t="s">
-        <v>392</v>
+        <v>385</v>
       </c>
       <c r="E94" s="4" t="s">
-        <v>454</v>
+        <v>446</v>
       </c>
     </row>
     <row r="95" spans="1:5" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A95" s="4" t="s">
-        <v>393</v>
+        <v>386</v>
       </c>
       <c r="B95" s="4" t="str">
         <f>VLOOKUP(A95,TableNames!$A$2:$B$12,2,FALSE)</f>
@@ -3796,15 +3775,15 @@
         <v>1</v>
       </c>
       <c r="D95" s="4" t="s">
-        <v>394</v>
+        <v>486</v>
       </c>
       <c r="E95" s="4" t="s">
-        <v>419</v>
+        <v>411</v>
       </c>
     </row>
     <row r="96" spans="1:5" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A96" s="4" t="s">
-        <v>393</v>
+        <v>386</v>
       </c>
       <c r="B96" s="4" t="str">
         <f>VLOOKUP(A96,TableNames!$A$2:$B$12,2,FALSE)</f>
@@ -3817,12 +3796,12 @@
         <v>309</v>
       </c>
       <c r="E96" s="4" t="s">
-        <v>403</v>
+        <v>395</v>
       </c>
     </row>
     <row r="97" spans="1:5" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A97" s="4" t="s">
-        <v>393</v>
+        <v>386</v>
       </c>
       <c r="B97" s="4" t="str">
         <f>VLOOKUP(A97,TableNames!$A$2:$B$12,2,FALSE)</f>
@@ -3832,15 +3811,15 @@
         <v>3</v>
       </c>
       <c r="D97" s="4" t="s">
-        <v>395</v>
+        <v>387</v>
       </c>
       <c r="E97" s="4" t="s">
-        <v>471</v>
+        <v>463</v>
       </c>
     </row>
     <row r="98" spans="1:5" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A98" s="4" t="s">
-        <v>393</v>
+        <v>386</v>
       </c>
       <c r="B98" s="4" t="str">
         <f>VLOOKUP(A98,TableNames!$A$2:$B$12,2,FALSE)</f>
@@ -3850,7 +3829,7 @@
         <v>4</v>
       </c>
       <c r="D98" s="4" t="s">
-        <v>396</v>
+        <v>388</v>
       </c>
       <c r="E98" s="4" t="s">
         <v>280</v>
@@ -3858,7 +3837,7 @@
     </row>
     <row r="99" spans="1:5" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A99" s="4" t="s">
-        <v>393</v>
+        <v>386</v>
       </c>
       <c r="B99" s="4" t="str">
         <f>VLOOKUP(A99,TableNames!$A$2:$B$12,2,FALSE)</f>
@@ -3868,15 +3847,15 @@
         <v>5</v>
       </c>
       <c r="D99" s="4" t="s">
-        <v>397</v>
+        <v>389</v>
       </c>
       <c r="E99" s="4" t="s">
-        <v>449</v>
+        <v>441</v>
       </c>
     </row>
     <row r="100" spans="1:5" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A100" s="4" t="s">
-        <v>393</v>
+        <v>386</v>
       </c>
       <c r="B100" s="4" t="str">
         <f>VLOOKUP(A100,TableNames!$A$2:$B$12,2,FALSE)</f>
@@ -3886,15 +3865,15 @@
         <v>6</v>
       </c>
       <c r="D100" s="4" t="s">
-        <v>398</v>
+        <v>390</v>
       </c>
       <c r="E100" s="4" t="s">
-        <v>450</v>
+        <v>442</v>
       </c>
     </row>
     <row r="101" spans="1:5" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A101" s="4" t="s">
-        <v>393</v>
+        <v>386</v>
       </c>
       <c r="B101" s="4" t="str">
         <f>VLOOKUP(A101,TableNames!$A$2:$B$12,2,FALSE)</f>
@@ -3904,15 +3883,15 @@
         <v>7</v>
       </c>
       <c r="D101" s="4" t="s">
-        <v>399</v>
+        <v>391</v>
       </c>
       <c r="E101" s="4" t="s">
-        <v>451</v>
+        <v>443</v>
       </c>
     </row>
     <row r="102" spans="1:5" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A102" s="4" t="s">
-        <v>393</v>
+        <v>386</v>
       </c>
       <c r="B102" s="4" t="str">
         <f>VLOOKUP(A102,TableNames!$A$2:$B$12,2,FALSE)</f>
@@ -3922,15 +3901,15 @@
         <v>8</v>
       </c>
       <c r="D102" s="4" t="s">
-        <v>400</v>
+        <v>392</v>
       </c>
       <c r="E102" s="4" t="s">
-        <v>452</v>
+        <v>444</v>
       </c>
     </row>
     <row r="103" spans="1:5" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A103" s="4" t="s">
-        <v>393</v>
+        <v>386</v>
       </c>
       <c r="B103" s="4" t="str">
         <f>VLOOKUP(A103,TableNames!$A$2:$B$12,2,FALSE)</f>
@@ -3940,10 +3919,10 @@
         <v>9</v>
       </c>
       <c r="D103" s="4" t="s">
-        <v>401</v>
+        <v>393</v>
       </c>
       <c r="E103" s="4" t="s">
-        <v>453</v>
+        <v>445</v>
       </c>
     </row>
   </sheetData>
@@ -3956,7 +3935,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6EF1C1D3-3AE0-4822-BECE-5F11FDFA805B}">
   <dimension ref="A1:L256"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="79" workbookViewId="0">
+    <sheetView zoomScale="79" workbookViewId="0">
       <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
@@ -3981,25 +3960,25 @@
   <sheetData>
     <row r="1" spans="1:8" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="3" t="s">
-        <v>493</v>
+        <v>485</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>492</v>
+        <v>484</v>
       </c>
       <c r="C1" s="3" t="s">
         <v>193</v>
       </c>
       <c r="D1" s="3" t="s">
-        <v>460</v>
+        <v>452</v>
       </c>
       <c r="E1" s="3" t="s">
-        <v>463</v>
+        <v>455</v>
       </c>
       <c r="F1" s="7" t="s">
-        <v>464</v>
+        <v>456</v>
       </c>
       <c r="G1" s="2" t="s">
-        <v>461</v>
+        <v>453</v>
       </c>
       <c r="H1" s="3" t="s">
         <v>194</v>
@@ -7762,13 +7741,13 @@
         <v>195</v>
       </c>
       <c r="D159" s="4" t="s">
-        <v>476</v>
+        <v>468</v>
       </c>
       <c r="E159" s="4" t="s">
-        <v>476</v>
+        <v>468</v>
       </c>
       <c r="F159" s="8" t="s">
-        <v>477</v>
+        <v>469</v>
       </c>
     </row>
     <row r="160" spans="1:8" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
@@ -8764,13 +8743,13 @@
         <v>195</v>
       </c>
       <c r="D201" s="4" t="s">
-        <v>474</v>
+        <v>466</v>
       </c>
       <c r="E201" s="4" t="s">
-        <v>474</v>
+        <v>466</v>
       </c>
       <c r="F201" s="8" t="s">
-        <v>475</v>
+        <v>467</v>
       </c>
       <c r="J201" s="5"/>
     </row>
@@ -9593,7 +9572,7 @@
         <v>261</v>
       </c>
       <c r="F236" s="8" t="s">
-        <v>489</v>
+        <v>481</v>
       </c>
       <c r="G236" s="5" t="s">
         <v>262</v>
@@ -10042,7 +10021,7 @@
         <v>46</v>
       </c>
       <c r="F253" s="9" t="s">
-        <v>488</v>
+        <v>480</v>
       </c>
       <c r="G253" s="5"/>
       <c r="J253" s="5"/>

</xml_diff>

<commit_message>
Temporary working output dsAugmentData
</commit_message>
<xml_diff>
--- a/Development/Data/MetaData/MetaDataCCP.xlsx
+++ b/Development/Data/MetaData/MetaDataCCP.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Basti\ARBEIT Lokal\dsCCPhos\Development\Data\MetaData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{78123EA3-432A-4D42-A4E1-C9910236EA1F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{888BD4D6-40E1-4C2A-8C86-6B2BD0F2F6B4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="16776" activeTab="1" xr2:uid="{035133D3-9E9F-4CDB-BCDC-A149BB1E9383}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1237" uniqueCount="487">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1237" uniqueCount="486">
   <si>
     <t>D</t>
   </si>
@@ -1181,9 +1181,6 @@
     <t>molecular-marker</t>
   </si>
   <si>
-    <t>mol-marker-id</t>
-  </si>
-  <si>
     <t>marker_datum</t>
   </si>
   <si>
@@ -1280,9 +1277,6 @@
     <t>ICDOMorphologyCode</t>
   </si>
   <si>
-    <t>TNMID</t>
-  </si>
-  <si>
     <t>TNM_rSymbol</t>
   </si>
   <si>
@@ -1497,6 +1491,9 @@
   </si>
   <si>
     <t>_id</t>
+  </si>
+  <si>
+    <t>StagingID</t>
   </si>
 </sst>
 </file>
@@ -1948,15 +1945,15 @@
   <sheetData>
     <row r="1" spans="1:2" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="3" t="s">
-        <v>447</v>
+        <v>445</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>454</v>
+        <v>452</v>
       </c>
     </row>
     <row r="2" spans="1:2" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="4" t="s">
-        <v>386</v>
+        <v>385</v>
       </c>
       <c r="B2" s="4" t="s">
         <v>277</v>
@@ -1991,7 +1988,7 @@
         <v>380</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>449</v>
+        <v>447</v>
       </c>
     </row>
     <row r="7" spans="1:2" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
@@ -1999,7 +1996,7 @@
         <v>308</v>
       </c>
       <c r="B7" s="4" t="s">
-        <v>451</v>
+        <v>449</v>
       </c>
     </row>
     <row r="8" spans="1:2" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
@@ -2015,7 +2012,7 @@
         <v>375</v>
       </c>
       <c r="B9" s="4" t="s">
-        <v>448</v>
+        <v>446</v>
       </c>
     </row>
     <row r="10" spans="1:2" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
@@ -2039,7 +2036,7 @@
         <v>357</v>
       </c>
       <c r="B12" s="4" t="s">
-        <v>419</v>
+        <v>417</v>
       </c>
     </row>
   </sheetData>
@@ -2055,8 +2052,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CD8BF945-9186-40D3-A998-0B845CD0DDFC}">
   <dimension ref="A1:E103"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A85" workbookViewId="0">
-      <selection activeCell="F92" sqref="F92"/>
+    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
+      <selection activeCell="E44" sqref="E44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="16.33203125" defaultRowHeight="25.2" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -2074,19 +2071,19 @@
   <sheetData>
     <row r="1" spans="1:5" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="3" t="s">
-        <v>447</v>
+        <v>445</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>454</v>
+        <v>452</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>394</v>
+        <v>393</v>
       </c>
       <c r="D1" s="3" t="s">
-        <v>450</v>
+        <v>448</v>
       </c>
       <c r="E1" s="3" t="s">
-        <v>457</v>
+        <v>455</v>
       </c>
     </row>
     <row r="2" spans="1:5" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
@@ -2101,10 +2098,10 @@
         <v>1</v>
       </c>
       <c r="D2" s="4" t="s">
-        <v>486</v>
+        <v>484</v>
       </c>
       <c r="E2" s="4" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
     </row>
     <row r="3" spans="1:5" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
@@ -2122,7 +2119,7 @@
         <v>310</v>
       </c>
       <c r="E3" s="4" t="s">
-        <v>397</v>
+        <v>396</v>
       </c>
     </row>
     <row r="4" spans="1:5" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
@@ -2140,7 +2137,7 @@
         <v>311</v>
       </c>
       <c r="E4" s="4" t="s">
-        <v>398</v>
+        <v>397</v>
       </c>
     </row>
     <row r="5" spans="1:5" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
@@ -2158,7 +2155,7 @@
         <v>312</v>
       </c>
       <c r="E5" s="4" t="s">
-        <v>399</v>
+        <v>398</v>
       </c>
     </row>
     <row r="6" spans="1:5" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
@@ -2176,7 +2173,7 @@
         <v>313</v>
       </c>
       <c r="E6" s="4" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
     </row>
     <row r="7" spans="1:5" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
@@ -2194,7 +2191,7 @@
         <v>314</v>
       </c>
       <c r="E7" s="4" t="s">
-        <v>460</v>
+        <v>458</v>
       </c>
     </row>
     <row r="8" spans="1:5" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
@@ -2230,7 +2227,7 @@
         <v>316</v>
       </c>
       <c r="E9" s="4" t="s">
-        <v>401</v>
+        <v>400</v>
       </c>
     </row>
     <row r="10" spans="1:5" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
@@ -2248,7 +2245,7 @@
         <v>317</v>
       </c>
       <c r="E10" s="4" t="s">
-        <v>402</v>
+        <v>401</v>
       </c>
     </row>
     <row r="11" spans="1:5" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
@@ -2263,10 +2260,10 @@
         <v>1</v>
       </c>
       <c r="D11" s="4" t="s">
-        <v>486</v>
+        <v>484</v>
       </c>
       <c r="E11" s="4" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
     </row>
     <row r="12" spans="1:5" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
@@ -2284,7 +2281,7 @@
         <v>309</v>
       </c>
       <c r="E12" s="4" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
     </row>
     <row r="13" spans="1:5" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
@@ -2302,7 +2299,7 @@
         <v>320</v>
       </c>
       <c r="E13" s="4" t="s">
-        <v>406</v>
+        <v>405</v>
       </c>
     </row>
     <row r="14" spans="1:5" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
@@ -2320,7 +2317,7 @@
         <v>321</v>
       </c>
       <c r="E14" s="4" t="s">
-        <v>471</v>
+        <v>469</v>
       </c>
     </row>
     <row r="15" spans="1:5" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
@@ -2338,7 +2335,7 @@
         <v>322</v>
       </c>
       <c r="E15" s="4" t="s">
-        <v>472</v>
+        <v>470</v>
       </c>
     </row>
     <row r="16" spans="1:5" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
@@ -2356,7 +2353,7 @@
         <v>323</v>
       </c>
       <c r="E16" s="4" t="s">
-        <v>403</v>
+        <v>402</v>
       </c>
     </row>
     <row r="17" spans="1:5" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
@@ -2374,7 +2371,7 @@
         <v>324</v>
       </c>
       <c r="E17" s="4" t="s">
-        <v>405</v>
+        <v>404</v>
       </c>
     </row>
     <row r="18" spans="1:5" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
@@ -2392,7 +2389,7 @@
         <v>325</v>
       </c>
       <c r="E18" s="4" t="s">
-        <v>404</v>
+        <v>403</v>
       </c>
     </row>
     <row r="19" spans="1:5" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
@@ -2425,10 +2422,10 @@
         <v>1</v>
       </c>
       <c r="D20" s="4" t="s">
-        <v>486</v>
+        <v>484</v>
       </c>
       <c r="E20" s="4" t="s">
-        <v>407</v>
+        <v>406</v>
       </c>
     </row>
     <row r="21" spans="1:5" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
@@ -2446,7 +2443,7 @@
         <v>319</v>
       </c>
       <c r="E21" s="4" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
     </row>
     <row r="22" spans="1:5" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
@@ -2464,7 +2461,7 @@
         <v>309</v>
       </c>
       <c r="E22" s="4" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
     </row>
     <row r="23" spans="1:5" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
@@ -2482,7 +2479,7 @@
         <v>328</v>
       </c>
       <c r="E23" s="4" t="s">
-        <v>470</v>
+        <v>468</v>
       </c>
     </row>
     <row r="24" spans="1:5" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
@@ -2500,7 +2497,7 @@
         <v>329</v>
       </c>
       <c r="E24" s="4" t="s">
-        <v>461</v>
+        <v>459</v>
       </c>
     </row>
     <row r="25" spans="1:5" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
@@ -2518,7 +2515,7 @@
         <v>330</v>
       </c>
       <c r="E25" s="4" t="s">
-        <v>479</v>
+        <v>477</v>
       </c>
     </row>
     <row r="26" spans="1:5" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
@@ -2536,7 +2533,7 @@
         <v>331</v>
       </c>
       <c r="E26" s="4" t="s">
-        <v>473</v>
+        <v>471</v>
       </c>
     </row>
     <row r="27" spans="1:5" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
@@ -2554,7 +2551,7 @@
         <v>332</v>
       </c>
       <c r="E27" s="4" t="s">
-        <v>474</v>
+        <v>472</v>
       </c>
     </row>
     <row r="28" spans="1:5" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
@@ -2572,7 +2569,7 @@
         <v>333</v>
       </c>
       <c r="E28" s="4" t="s">
-        <v>475</v>
+        <v>473</v>
       </c>
     </row>
     <row r="29" spans="1:5" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
@@ -2587,10 +2584,10 @@
         <v>1</v>
       </c>
       <c r="D29" s="4" t="s">
-        <v>486</v>
+        <v>484</v>
       </c>
       <c r="E29" s="4" t="s">
-        <v>408</v>
+        <v>407</v>
       </c>
     </row>
     <row r="30" spans="1:5" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
@@ -2608,7 +2605,7 @@
         <v>319</v>
       </c>
       <c r="E30" s="4" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
     </row>
     <row r="31" spans="1:5" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
@@ -2626,7 +2623,7 @@
         <v>309</v>
       </c>
       <c r="E31" s="4" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
     </row>
     <row r="32" spans="1:5" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
@@ -2644,7 +2641,7 @@
         <v>335</v>
       </c>
       <c r="E32" s="4" t="s">
-        <v>462</v>
+        <v>460</v>
       </c>
     </row>
     <row r="33" spans="1:5" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
@@ -2662,7 +2659,7 @@
         <v>336</v>
       </c>
       <c r="E33" s="4" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
     </row>
     <row r="34" spans="1:5" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
@@ -2680,7 +2677,7 @@
         <v>337</v>
       </c>
       <c r="E34" s="4" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
     </row>
     <row r="35" spans="1:5" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
@@ -2698,7 +2695,7 @@
         <v>338</v>
       </c>
       <c r="E35" s="4" t="s">
-        <v>482</v>
+        <v>480</v>
       </c>
     </row>
     <row r="36" spans="1:5" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
@@ -2731,10 +2728,10 @@
         <v>1</v>
       </c>
       <c r="D37" s="4" t="s">
-        <v>486</v>
+        <v>484</v>
       </c>
       <c r="E37" s="4" t="s">
-        <v>409</v>
+        <v>408</v>
       </c>
     </row>
     <row r="38" spans="1:5" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
@@ -2752,7 +2749,7 @@
         <v>319</v>
       </c>
       <c r="E38" s="4" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
     </row>
     <row r="39" spans="1:5" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
@@ -2770,7 +2767,7 @@
         <v>309</v>
       </c>
       <c r="E39" s="4" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
     </row>
     <row r="40" spans="1:5" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
@@ -2788,7 +2785,7 @@
         <v>341</v>
       </c>
       <c r="E40" s="4" t="s">
-        <v>459</v>
+        <v>457</v>
       </c>
     </row>
     <row r="41" spans="1:5" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
@@ -2806,7 +2803,7 @@
         <v>342</v>
       </c>
       <c r="E41" s="4" t="s">
-        <v>476</v>
+        <v>474</v>
       </c>
     </row>
     <row r="42" spans="1:5" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
@@ -2824,7 +2821,7 @@
         <v>343</v>
       </c>
       <c r="E42" s="4" t="s">
-        <v>477</v>
+        <v>475</v>
       </c>
     </row>
     <row r="43" spans="1:5" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
@@ -2839,10 +2836,10 @@
         <v>1</v>
       </c>
       <c r="D43" s="4" t="s">
-        <v>486</v>
+        <v>484</v>
       </c>
       <c r="E43" s="4" t="s">
-        <v>414</v>
+        <v>485</v>
       </c>
     </row>
     <row r="44" spans="1:5" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
@@ -2860,7 +2857,7 @@
         <v>319</v>
       </c>
       <c r="E44" s="4" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
     </row>
     <row r="45" spans="1:5" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
@@ -2878,7 +2875,7 @@
         <v>309</v>
       </c>
       <c r="E45" s="4" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
     </row>
     <row r="46" spans="1:5" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
@@ -2896,7 +2893,7 @@
         <v>345</v>
       </c>
       <c r="E46" s="4" t="s">
-        <v>478</v>
+        <v>476</v>
       </c>
     </row>
     <row r="47" spans="1:5" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
@@ -3040,7 +3037,7 @@
         <v>353</v>
       </c>
       <c r="E54" s="4" t="s">
-        <v>465</v>
+        <v>463</v>
       </c>
     </row>
     <row r="55" spans="1:5" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
@@ -3058,7 +3055,7 @@
         <v>354</v>
       </c>
       <c r="E55" s="4" t="s">
-        <v>415</v>
+        <v>413</v>
       </c>
     </row>
     <row r="56" spans="1:5" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
@@ -3076,7 +3073,7 @@
         <v>355</v>
       </c>
       <c r="E56" s="4" t="s">
-        <v>416</v>
+        <v>414</v>
       </c>
     </row>
     <row r="57" spans="1:5" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
@@ -3094,7 +3091,7 @@
         <v>356</v>
       </c>
       <c r="E57" s="4" t="s">
-        <v>417</v>
+        <v>415</v>
       </c>
     </row>
     <row r="58" spans="1:5" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
@@ -3109,10 +3106,10 @@
         <v>1</v>
       </c>
       <c r="D58" s="4" t="s">
-        <v>486</v>
+        <v>484</v>
       </c>
       <c r="E58" s="4" t="s">
-        <v>418</v>
+        <v>416</v>
       </c>
     </row>
     <row r="59" spans="1:5" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
@@ -3130,7 +3127,7 @@
         <v>319</v>
       </c>
       <c r="E59" s="4" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
     </row>
     <row r="60" spans="1:5" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
@@ -3148,7 +3145,7 @@
         <v>309</v>
       </c>
       <c r="E60" s="4" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
     </row>
     <row r="61" spans="1:5" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
@@ -3163,10 +3160,10 @@
         <v>4</v>
       </c>
       <c r="D61" s="4" t="s">
-        <v>483</v>
+        <v>481</v>
       </c>
       <c r="E61" s="4" t="s">
-        <v>431</v>
+        <v>429</v>
       </c>
     </row>
     <row r="62" spans="1:5" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
@@ -3184,7 +3181,7 @@
         <v>358</v>
       </c>
       <c r="E62" s="4" t="s">
-        <v>464</v>
+        <v>462</v>
       </c>
     </row>
     <row r="63" spans="1:5" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
@@ -3202,7 +3199,7 @@
         <v>359</v>
       </c>
       <c r="E63" s="4" t="s">
-        <v>420</v>
+        <v>418</v>
       </c>
     </row>
     <row r="64" spans="1:5" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
@@ -3220,7 +3217,7 @@
         <v>360</v>
       </c>
       <c r="E64" s="4" t="s">
-        <v>421</v>
+        <v>419</v>
       </c>
     </row>
     <row r="65" spans="1:5" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
@@ -3238,7 +3235,7 @@
         <v>361</v>
       </c>
       <c r="E65" s="4" t="s">
-        <v>422</v>
+        <v>420</v>
       </c>
     </row>
     <row r="66" spans="1:5" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
@@ -3256,7 +3253,7 @@
         <v>362</v>
       </c>
       <c r="E66" s="4" t="s">
-        <v>423</v>
+        <v>421</v>
       </c>
     </row>
     <row r="67" spans="1:5" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
@@ -3274,7 +3271,7 @@
         <v>363</v>
       </c>
       <c r="E67" s="4" t="s">
-        <v>424</v>
+        <v>422</v>
       </c>
     </row>
     <row r="68" spans="1:5" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
@@ -3292,7 +3289,7 @@
         <v>364</v>
       </c>
       <c r="E68" s="4" t="s">
-        <v>425</v>
+        <v>423</v>
       </c>
     </row>
     <row r="69" spans="1:5" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
@@ -3310,7 +3307,7 @@
         <v>365</v>
       </c>
       <c r="E69" s="4" t="s">
-        <v>458</v>
+        <v>456</v>
       </c>
     </row>
     <row r="70" spans="1:5" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
@@ -3328,7 +3325,7 @@
         <v>366</v>
       </c>
       <c r="E70" s="4" t="s">
-        <v>426</v>
+        <v>424</v>
       </c>
     </row>
     <row r="71" spans="1:5" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
@@ -3346,7 +3343,7 @@
         <v>367</v>
       </c>
       <c r="E71" s="4" t="s">
-        <v>427</v>
+        <v>425</v>
       </c>
     </row>
     <row r="72" spans="1:5" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
@@ -3364,7 +3361,7 @@
         <v>368</v>
       </c>
       <c r="E72" s="4" t="s">
-        <v>428</v>
+        <v>426</v>
       </c>
     </row>
     <row r="73" spans="1:5" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
@@ -3379,10 +3376,10 @@
         <v>1</v>
       </c>
       <c r="D73" s="4" t="s">
-        <v>486</v>
+        <v>484</v>
       </c>
       <c r="E73" s="4" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
     </row>
     <row r="74" spans="1:5" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
@@ -3400,7 +3397,7 @@
         <v>319</v>
       </c>
       <c r="E74" s="4" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
     </row>
     <row r="75" spans="1:5" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
@@ -3418,7 +3415,7 @@
         <v>309</v>
       </c>
       <c r="E75" s="4" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
     </row>
     <row r="76" spans="1:5" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
@@ -3436,7 +3433,7 @@
         <v>370</v>
       </c>
       <c r="E76" s="4" t="s">
-        <v>429</v>
+        <v>427</v>
       </c>
     </row>
     <row r="77" spans="1:5" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
@@ -3454,7 +3451,7 @@
         <v>371</v>
       </c>
       <c r="E77" s="4" t="s">
-        <v>430</v>
+        <v>428</v>
       </c>
     </row>
     <row r="78" spans="1:5" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
@@ -3523,10 +3520,10 @@
         <v>1</v>
       </c>
       <c r="D81" s="4" t="s">
-        <v>486</v>
+        <v>484</v>
       </c>
       <c r="E81" s="4" t="s">
-        <v>432</v>
+        <v>430</v>
       </c>
     </row>
     <row r="82" spans="1:5" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
@@ -3544,7 +3541,7 @@
         <v>319</v>
       </c>
       <c r="E82" s="4" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
     </row>
     <row r="83" spans="1:5" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
@@ -3562,7 +3559,7 @@
         <v>309</v>
       </c>
       <c r="E83" s="4" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
     </row>
     <row r="84" spans="1:5" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
@@ -3580,7 +3577,7 @@
         <v>376</v>
       </c>
       <c r="E84" s="4" t="s">
-        <v>433</v>
+        <v>431</v>
       </c>
     </row>
     <row r="85" spans="1:5" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
@@ -3598,7 +3595,7 @@
         <v>377</v>
       </c>
       <c r="E85" s="4" t="s">
-        <v>434</v>
+        <v>432</v>
       </c>
     </row>
     <row r="86" spans="1:5" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
@@ -3616,7 +3613,7 @@
         <v>378</v>
       </c>
       <c r="E86" s="4" t="s">
-        <v>435</v>
+        <v>433</v>
       </c>
     </row>
     <row r="87" spans="1:5" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
@@ -3634,7 +3631,7 @@
         <v>379</v>
       </c>
       <c r="E87" s="4" t="s">
-        <v>436</v>
+        <v>434</v>
       </c>
     </row>
     <row r="88" spans="1:5" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
@@ -3649,10 +3646,10 @@
         <v>1</v>
       </c>
       <c r="D88" s="4" t="s">
-        <v>381</v>
+        <v>484</v>
       </c>
       <c r="E88" s="4" t="s">
-        <v>437</v>
+        <v>435</v>
       </c>
     </row>
     <row r="89" spans="1:5" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
@@ -3670,7 +3667,7 @@
         <v>319</v>
       </c>
       <c r="E89" s="4" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
     </row>
     <row r="90" spans="1:5" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
@@ -3688,7 +3685,7 @@
         <v>309</v>
       </c>
       <c r="E90" s="4" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
     </row>
     <row r="91" spans="1:5" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
@@ -3703,10 +3700,10 @@
         <v>4</v>
       </c>
       <c r="D91" s="4" t="s">
-        <v>382</v>
+        <v>381</v>
       </c>
       <c r="E91" s="4" t="s">
-        <v>438</v>
+        <v>436</v>
       </c>
     </row>
     <row r="92" spans="1:5" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
@@ -3721,10 +3718,10 @@
         <v>5</v>
       </c>
       <c r="D92" s="4" t="s">
-        <v>383</v>
+        <v>382</v>
       </c>
       <c r="E92" s="4" t="s">
-        <v>439</v>
+        <v>437</v>
       </c>
     </row>
     <row r="93" spans="1:5" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
@@ -3739,10 +3736,10 @@
         <v>6</v>
       </c>
       <c r="D93" s="4" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
       <c r="E93" s="4" t="s">
-        <v>440</v>
+        <v>438</v>
       </c>
     </row>
     <row r="94" spans="1:5" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
@@ -3757,15 +3754,15 @@
         <v>7</v>
       </c>
       <c r="D94" s="4" t="s">
-        <v>385</v>
+        <v>384</v>
       </c>
       <c r="E94" s="4" t="s">
-        <v>446</v>
+        <v>444</v>
       </c>
     </row>
     <row r="95" spans="1:5" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A95" s="4" t="s">
-        <v>386</v>
+        <v>385</v>
       </c>
       <c r="B95" s="4" t="str">
         <f>VLOOKUP(A95,TableNames!$A$2:$B$12,2,FALSE)</f>
@@ -3775,15 +3772,15 @@
         <v>1</v>
       </c>
       <c r="D95" s="4" t="s">
-        <v>486</v>
+        <v>484</v>
       </c>
       <c r="E95" s="4" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
     </row>
     <row r="96" spans="1:5" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A96" s="4" t="s">
-        <v>386</v>
+        <v>385</v>
       </c>
       <c r="B96" s="4" t="str">
         <f>VLOOKUP(A96,TableNames!$A$2:$B$12,2,FALSE)</f>
@@ -3796,12 +3793,12 @@
         <v>309</v>
       </c>
       <c r="E96" s="4" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
     </row>
     <row r="97" spans="1:5" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A97" s="4" t="s">
-        <v>386</v>
+        <v>385</v>
       </c>
       <c r="B97" s="4" t="str">
         <f>VLOOKUP(A97,TableNames!$A$2:$B$12,2,FALSE)</f>
@@ -3811,15 +3808,15 @@
         <v>3</v>
       </c>
       <c r="D97" s="4" t="s">
-        <v>387</v>
+        <v>386</v>
       </c>
       <c r="E97" s="4" t="s">
-        <v>463</v>
+        <v>461</v>
       </c>
     </row>
     <row r="98" spans="1:5" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A98" s="4" t="s">
-        <v>386</v>
+        <v>385</v>
       </c>
       <c r="B98" s="4" t="str">
         <f>VLOOKUP(A98,TableNames!$A$2:$B$12,2,FALSE)</f>
@@ -3829,7 +3826,7 @@
         <v>4</v>
       </c>
       <c r="D98" s="4" t="s">
-        <v>388</v>
+        <v>387</v>
       </c>
       <c r="E98" s="4" t="s">
         <v>280</v>
@@ -3837,7 +3834,7 @@
     </row>
     <row r="99" spans="1:5" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A99" s="4" t="s">
-        <v>386</v>
+        <v>385</v>
       </c>
       <c r="B99" s="4" t="str">
         <f>VLOOKUP(A99,TableNames!$A$2:$B$12,2,FALSE)</f>
@@ -3847,15 +3844,15 @@
         <v>5</v>
       </c>
       <c r="D99" s="4" t="s">
-        <v>389</v>
+        <v>388</v>
       </c>
       <c r="E99" s="4" t="s">
-        <v>441</v>
+        <v>439</v>
       </c>
     </row>
     <row r="100" spans="1:5" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A100" s="4" t="s">
-        <v>386</v>
+        <v>385</v>
       </c>
       <c r="B100" s="4" t="str">
         <f>VLOOKUP(A100,TableNames!$A$2:$B$12,2,FALSE)</f>
@@ -3865,15 +3862,15 @@
         <v>6</v>
       </c>
       <c r="D100" s="4" t="s">
-        <v>390</v>
+        <v>389</v>
       </c>
       <c r="E100" s="4" t="s">
-        <v>442</v>
+        <v>440</v>
       </c>
     </row>
     <row r="101" spans="1:5" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A101" s="4" t="s">
-        <v>386</v>
+        <v>385</v>
       </c>
       <c r="B101" s="4" t="str">
         <f>VLOOKUP(A101,TableNames!$A$2:$B$12,2,FALSE)</f>
@@ -3883,15 +3880,15 @@
         <v>7</v>
       </c>
       <c r="D101" s="4" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
       <c r="E101" s="4" t="s">
-        <v>443</v>
+        <v>441</v>
       </c>
     </row>
     <row r="102" spans="1:5" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A102" s="4" t="s">
-        <v>386</v>
+        <v>385</v>
       </c>
       <c r="B102" s="4" t="str">
         <f>VLOOKUP(A102,TableNames!$A$2:$B$12,2,FALSE)</f>
@@ -3901,15 +3898,15 @@
         <v>8</v>
       </c>
       <c r="D102" s="4" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
       <c r="E102" s="4" t="s">
-        <v>444</v>
+        <v>442</v>
       </c>
     </row>
     <row r="103" spans="1:5" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A103" s="4" t="s">
-        <v>386</v>
+        <v>385</v>
       </c>
       <c r="B103" s="4" t="str">
         <f>VLOOKUP(A103,TableNames!$A$2:$B$12,2,FALSE)</f>
@@ -3919,10 +3916,10 @@
         <v>9</v>
       </c>
       <c r="D103" s="4" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
       <c r="E103" s="4" t="s">
-        <v>445</v>
+        <v>443</v>
       </c>
     </row>
   </sheetData>
@@ -3960,25 +3957,25 @@
   <sheetData>
     <row r="1" spans="1:8" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="3" t="s">
-        <v>485</v>
+        <v>483</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>484</v>
+        <v>482</v>
       </c>
       <c r="C1" s="3" t="s">
         <v>193</v>
       </c>
       <c r="D1" s="3" t="s">
-        <v>452</v>
+        <v>450</v>
       </c>
       <c r="E1" s="3" t="s">
-        <v>455</v>
+        <v>453</v>
       </c>
       <c r="F1" s="7" t="s">
-        <v>456</v>
+        <v>454</v>
       </c>
       <c r="G1" s="2" t="s">
-        <v>453</v>
+        <v>451</v>
       </c>
       <c r="H1" s="3" t="s">
         <v>194</v>
@@ -7741,13 +7738,13 @@
         <v>195</v>
       </c>
       <c r="D159" s="4" t="s">
-        <v>468</v>
+        <v>466</v>
       </c>
       <c r="E159" s="4" t="s">
-        <v>468</v>
+        <v>466</v>
       </c>
       <c r="F159" s="8" t="s">
-        <v>469</v>
+        <v>467</v>
       </c>
     </row>
     <row r="160" spans="1:8" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
@@ -8743,13 +8740,13 @@
         <v>195</v>
       </c>
       <c r="D201" s="4" t="s">
-        <v>466</v>
+        <v>464</v>
       </c>
       <c r="E201" s="4" t="s">
-        <v>466</v>
+        <v>464</v>
       </c>
       <c r="F201" s="8" t="s">
-        <v>467</v>
+        <v>465</v>
       </c>
       <c r="J201" s="5"/>
     </row>
@@ -9572,7 +9569,7 @@
         <v>261</v>
       </c>
       <c r="F236" s="8" t="s">
-        <v>481</v>
+        <v>479</v>
       </c>
       <c r="G236" s="5" t="s">
         <v>262</v>
@@ -10021,7 +10018,7 @@
         <v>46</v>
       </c>
       <c r="F253" s="9" t="s">
-        <v>480</v>
+        <v>478</v>
       </c>
       <c r="G253" s="5"/>
       <c r="J253" s="5"/>

</xml_diff>

<commit_message>
Working on transformation monitoring
</commit_message>
<xml_diff>
--- a/Development/Data/MetaData/MetaDataCCP.xlsx
+++ b/Development/Data/MetaData/MetaDataCCP.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Basti\ARBEIT Lokal\dsCCPhos\Development\Data\MetaData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{888BD4D6-40E1-4C2A-8C86-6B2BD0F2F6B4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D716B253-7EAD-4DEB-BA5A-80233F4F2F59}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="16776" activeTab="1" xr2:uid="{035133D3-9E9F-4CDB-BCDC-A149BB1E9383}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="16776" activeTab="2" xr2:uid="{035133D3-9E9F-4CDB-BCDC-A149BB1E9383}"/>
   </bookViews>
   <sheets>
     <sheet name="TableNames" sheetId="11" r:id="rId1"/>
@@ -2052,7 +2052,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CD8BF945-9186-40D3-A998-0B845CD0DDFC}">
   <dimension ref="A1:E103"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E44" sqref="E44"/>
     </sheetView>
   </sheetViews>
@@ -3932,11 +3932,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6EF1C1D3-3AE0-4822-BECE-5F11FDFA805B}">
   <dimension ref="A1:L256"/>
   <sheetViews>
-    <sheetView zoomScale="79" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="79" workbookViewId="0">
       <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="B2" sqref="B2"/>
+      <selection pane="bottomRight" activeCell="K5" sqref="K5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="16.33203125" defaultRowHeight="25.2" customHeight="1" x14ac:dyDescent="0.3"/>

</xml_diff>